<commit_message>
<개발 일정 수정 22.08.19 ver>
- 개발 일정 중 내 옷장을 완성하기 전 페이지네이션 처리가 먼저 필요하다고 느껴서 페이지네이션 처리 구현 일정을 당기고, 내 옷장 구현을 뒤로 미룸
</commit_message>
<xml_diff>
--- a/개발일정/개발일정.xlsx
+++ b/개발일정/개발일정.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jeongbin\개발일정\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4C3BAE-E43A-4A6D-B442-CECC974E4065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B68A666-FFE0-4C3F-9989-D6F8C2C1F1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{35D19782-2640-4577-BDC1-AB3DBC55561F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{35D19782-2640-4577-BDC1-AB3DBC55561F}"/>
   </bookViews>
   <sheets>
     <sheet name="3월" sheetId="1" r:id="rId1"/>
@@ -1536,10 +1536,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>22.08.20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>9월 4일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1682,6 +1678,10 @@
   </si>
   <si>
     <t>22.09.30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22.08.23</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1880,7 +1880,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -2194,13 +2194,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2516,6 +2529,42 @@
     <xf numFmtId="0" fontId="5" fillId="19" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2594,100 +2643,55 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3060,12 +3064,12 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="110" t="s">
+      <c r="E5" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="112"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="124"/>
     </row>
     <row r="6" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
@@ -3091,17 +3095,17 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="105" t="s">
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="107"/>
+      <c r="H7" s="119"/>
     </row>
     <row r="8" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
@@ -3127,15 +3131,15 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="106"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="107"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="119"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
@@ -3161,14 +3165,14 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="107"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="119"/>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -3235,13 +3239,13 @@
       <c r="B1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="125" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
@@ -3318,12 +3322,12 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="108" t="s">
+      <c r="K6" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="109"/>
-      <c r="M6" s="109"/>
-      <c r="N6" s="117"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="129"/>
     </row>
     <row r="7" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="21">
@@ -3376,17 +3380,17 @@
         <v>19</v>
       </c>
       <c r="G9" s="32"/>
-      <c r="H9" s="108" t="s">
+      <c r="H9" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="105" t="s">
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="107"/>
+      <c r="N9" s="119"/>
     </row>
     <row r="10" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="21">
@@ -3862,10 +3866,10 @@
       <c r="L29" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="M29" s="105" t="s">
+      <c r="M29" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="N29" s="107"/>
+      <c r="N29" s="119"/>
     </row>
     <row r="30" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="21">
@@ -3966,13 +3970,13 @@
       <c r="G33" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="H33" s="105"/>
-      <c r="I33" s="106"/>
-      <c r="J33" s="106"/>
-      <c r="K33" s="106"/>
-      <c r="L33" s="106"/>
-      <c r="M33" s="106"/>
-      <c r="N33" s="107"/>
+      <c r="H33" s="117"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="118"/>
+      <c r="K33" s="118"/>
+      <c r="L33" s="118"/>
+      <c r="M33" s="118"/>
+      <c r="N33" s="119"/>
     </row>
     <row r="34" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21">
@@ -3988,13 +3992,13 @@
       <c r="G34" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="H34" s="114"/>
-      <c r="I34" s="115"/>
-      <c r="J34" s="115"/>
-      <c r="K34" s="115"/>
-      <c r="L34" s="115"/>
-      <c r="M34" s="115"/>
-      <c r="N34" s="116"/>
+      <c r="H34" s="126"/>
+      <c r="I34" s="127"/>
+      <c r="J34" s="127"/>
+      <c r="K34" s="127"/>
+      <c r="L34" s="127"/>
+      <c r="M34" s="127"/>
+      <c r="N34" s="128"/>
     </row>
     <row r="35" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21">
@@ -4059,15 +4063,15 @@
       <c r="G37" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="H37" s="105" t="s">
+      <c r="H37" s="117" t="s">
         <v>123</v>
       </c>
-      <c r="I37" s="106"/>
-      <c r="J37" s="106"/>
-      <c r="K37" s="106"/>
-      <c r="L37" s="106"/>
-      <c r="M37" s="106"/>
-      <c r="N37" s="107"/>
+      <c r="I37" s="118"/>
+      <c r="J37" s="118"/>
+      <c r="K37" s="118"/>
+      <c r="L37" s="118"/>
+      <c r="M37" s="118"/>
+      <c r="N37" s="119"/>
     </row>
     <row r="38" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="21">
@@ -4083,13 +4087,13 @@
       <c r="G38" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="H38" s="114"/>
-      <c r="I38" s="115"/>
-      <c r="J38" s="115"/>
-      <c r="K38" s="115"/>
-      <c r="L38" s="115"/>
-      <c r="M38" s="115"/>
-      <c r="N38" s="116"/>
+      <c r="H38" s="126"/>
+      <c r="I38" s="127"/>
+      <c r="J38" s="127"/>
+      <c r="K38" s="127"/>
+      <c r="L38" s="127"/>
+      <c r="M38" s="127"/>
+      <c r="N38" s="128"/>
     </row>
     <row r="39" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="21">
@@ -4708,13 +4712,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:12" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
     </row>
     <row r="3" spans="5:12" x14ac:dyDescent="0.3">
       <c r="F3" s="2" t="s">
@@ -4768,13 +4772,13 @@
       </c>
       <c r="F6" s="72"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="108" t="s">
+      <c r="H6" s="120" t="s">
         <v>157</v>
       </c>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="117"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="129"/>
     </row>
     <row r="7" spans="5:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F7" s="1"/>
@@ -4811,15 +4815,15 @@
       <c r="E9" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="F9" s="118" t="s">
+      <c r="F9" s="130" t="s">
         <v>161</v>
       </c>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="120"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="131"/>
+      <c r="J9" s="131"/>
+      <c r="K9" s="131"/>
+      <c r="L9" s="132"/>
     </row>
     <row r="10" spans="5:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E10" s="33"/>
@@ -4943,13 +4947,13 @@
         <v>158</v>
       </c>
       <c r="F18" s="67"/>
-      <c r="G18" s="105" t="s">
+      <c r="G18" s="117" t="s">
         <v>214</v>
       </c>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="106"/>
-      <c r="K18" s="106"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
       <c r="L18" s="53"/>
     </row>
   </sheetData>
@@ -4987,13 +4991,13 @@
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A1" s="55"/>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="125" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F3" s="2" t="s">
@@ -5045,11 +5049,11 @@
       </c>
       <c r="F6" s="72"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="125"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="136"/>
+      <c r="L6" s="137"/>
     </row>
     <row r="7" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F7" s="1"/>
@@ -5086,13 +5090,13 @@
       <c r="E9" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="F9" s="126"/>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="127"/>
-      <c r="J9" s="127"/>
-      <c r="K9" s="127"/>
-      <c r="L9" s="128"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="139"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="140"/>
     </row>
     <row r="10" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E10" s="33"/>
@@ -5462,8 +5466,8 @@
       <c r="G33" s="83"/>
       <c r="H33" s="82"/>
       <c r="I33" s="82"/>
-      <c r="J33" s="121"/>
-      <c r="K33" s="122"/>
+      <c r="J33" s="133"/>
+      <c r="K33" s="134"/>
       <c r="L33" s="85"/>
     </row>
   </sheetData>
@@ -5483,8 +5487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F9D2E6-B680-4670-861D-0722D511F357}">
   <dimension ref="D2:N36"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5496,13 +5500,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:11" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="F2" s="113" t="s">
+      <c r="F2" s="125" t="s">
         <v>304</v>
       </c>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E4" s="2" t="s">
@@ -5730,13 +5734,13 @@
       <c r="D20" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="E20" s="139"/>
-      <c r="F20" s="139"/>
-      <c r="G20" s="139"/>
-      <c r="H20" s="139"/>
-      <c r="I20" s="139"/>
-      <c r="J20" s="139"/>
-      <c r="K20" s="139"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
+      <c r="I20" s="106"/>
+      <c r="J20" s="106"/>
+      <c r="K20" s="106"/>
     </row>
     <row r="21" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="33"/>
@@ -5771,21 +5775,19 @@
       <c r="D23" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="E23" s="139"/>
-      <c r="F23" s="139"/>
-      <c r="G23" s="139"/>
-      <c r="H23" s="140" t="s">
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="109" t="s">
         <v>331</v>
       </c>
       <c r="I23" s="98" t="s">
         <v>331</v>
       </c>
-      <c r="J23" s="98" t="s">
-        <v>331</v>
-      </c>
-      <c r="K23" s="98" t="s">
-        <v>331</v>
-      </c>
+      <c r="J23" s="141" t="s">
+        <v>344</v>
+      </c>
+      <c r="K23" s="142"/>
     </row>
     <row r="24" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -5818,18 +5820,20 @@
       <c r="D26" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="129" t="s">
+      <c r="E26" s="141" t="s">
         <v>344</v>
       </c>
-      <c r="F26" s="130"/>
-      <c r="G26" s="130"/>
-      <c r="H26" s="130"/>
-      <c r="I26" s="130"/>
-      <c r="J26" s="130"/>
-      <c r="K26" s="130"/>
-      <c r="L26" s="156"/>
-      <c r="M26" s="146"/>
-      <c r="N26" s="146"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="142"/>
+      <c r="H26" s="158" t="s">
+        <v>331</v>
+      </c>
+      <c r="I26" s="158"/>
+      <c r="J26" s="158"/>
+      <c r="K26" s="159"/>
+      <c r="L26" s="115"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
     </row>
     <row r="27" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -5923,9 +5927,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="F2:J2"/>
-    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:K26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5953,13 +5959,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:14" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="I1" s="113" t="s">
+      <c r="I1" s="125" t="s">
         <v>362</v>
       </c>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
     </row>
     <row r="3" spans="7:14" x14ac:dyDescent="0.3">
       <c r="H3" s="2" t="s">
@@ -5992,25 +5998,25 @@
         <v>54</v>
       </c>
       <c r="H6" s="39" t="s">
+        <v>422</v>
+      </c>
+      <c r="I6" s="39" t="s">
         <v>423</v>
       </c>
-      <c r="I6" s="39" t="s">
+      <c r="J6" s="39" t="s">
         <v>424</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="K6" s="39" t="s">
         <v>425</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="L6" s="39" t="s">
         <v>426</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="M6" s="68" t="s">
         <v>427</v>
       </c>
-      <c r="M6" s="68" t="s">
+      <c r="N6" s="65" t="s">
         <v>428</v>
-      </c>
-      <c r="N6" s="65" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="7" spans="7:14" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6032,10 +6038,10 @@
       <c r="L7" s="103" t="s">
         <v>334</v>
       </c>
-      <c r="M7" s="157" t="s">
-        <v>457</v>
-      </c>
-      <c r="N7" s="158"/>
+      <c r="M7" s="147" t="s">
+        <v>456</v>
+      </c>
+      <c r="N7" s="148"/>
     </row>
     <row r="8" spans="7:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G8" s="33"/>
@@ -6045,40 +6051,40 @@
         <v>54</v>
       </c>
       <c r="H9" s="68" t="s">
+        <v>429</v>
+      </c>
+      <c r="I9" s="68" t="s">
         <v>430</v>
       </c>
-      <c r="I9" s="68" t="s">
+      <c r="J9" s="68" t="s">
         <v>431</v>
       </c>
-      <c r="J9" s="68" t="s">
+      <c r="K9" s="68" t="s">
         <v>432</v>
       </c>
-      <c r="K9" s="68" t="s">
+      <c r="L9" s="68" t="s">
         <v>433</v>
       </c>
-      <c r="L9" s="68" t="s">
+      <c r="M9" s="68" t="s">
         <v>434</v>
       </c>
-      <c r="M9" s="68" t="s">
+      <c r="N9" s="68" t="s">
         <v>435</v>
-      </c>
-      <c r="N9" s="68" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="10" spans="7:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G10" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="H10" s="162" t="s">
+      <c r="H10" s="116" t="s">
+        <v>456</v>
+      </c>
+      <c r="I10" s="144" t="s">
         <v>457</v>
       </c>
-      <c r="I10" s="159" t="s">
-        <v>458</v>
-      </c>
-      <c r="J10" s="160"/>
-      <c r="K10" s="160"/>
-      <c r="L10" s="161"/>
+      <c r="J10" s="145"/>
+      <c r="K10" s="145"/>
+      <c r="L10" s="146"/>
       <c r="M10" s="97" t="s">
         <v>335</v>
       </c>
@@ -6092,25 +6098,25 @@
         <v>54</v>
       </c>
       <c r="H12" s="39" t="s">
+        <v>436</v>
+      </c>
+      <c r="I12" s="39" t="s">
         <v>437</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="J12" s="39" t="s">
         <v>438</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="K12" s="39" t="s">
         <v>439</v>
       </c>
-      <c r="K12" s="39" t="s">
+      <c r="L12" s="39" t="s">
         <v>440</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="M12" s="39" t="s">
         <v>441</v>
       </c>
-      <c r="M12" s="39" t="s">
+      <c r="N12" s="39" t="s">
         <v>442</v>
-      </c>
-      <c r="N12" s="39" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="13" spans="7:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -6145,22 +6151,22 @@
         <v>54</v>
       </c>
       <c r="H15" s="39" t="s">
+        <v>443</v>
+      </c>
+      <c r="I15" s="39" t="s">
         <v>444</v>
       </c>
-      <c r="I15" s="39" t="s">
+      <c r="J15" s="39" t="s">
         <v>445</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="K15" s="39" t="s">
         <v>446</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="L15" s="39" t="s">
         <v>447</v>
       </c>
-      <c r="L15" s="39" t="s">
+      <c r="M15" s="39" t="s">
         <v>448</v>
-      </c>
-      <c r="M15" s="39" t="s">
-        <v>449</v>
       </c>
       <c r="N15" s="39"/>
     </row>
@@ -6168,98 +6174,70 @@
       <c r="G16" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="H16" s="154" t="s">
+      <c r="H16" s="149" t="s">
         <v>356</v>
       </c>
-      <c r="I16" s="155"/>
-      <c r="J16" s="155"/>
-      <c r="K16" s="155"/>
-      <c r="L16" s="155"/>
-      <c r="M16" s="155"/>
-      <c r="N16" s="138"/>
+      <c r="I16" s="150"/>
+      <c r="J16" s="150"/>
+      <c r="K16" s="150"/>
+      <c r="L16" s="150"/>
+      <c r="M16" s="150"/>
+      <c r="N16" s="108"/>
     </row>
     <row r="17" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G17" s="33"/>
     </row>
     <row r="18" spans="7:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="G18" s="141"/>
-      <c r="H18" s="142"/>
-      <c r="I18" s="142"/>
-      <c r="J18" s="142"/>
-      <c r="K18" s="142"/>
-      <c r="L18" s="142"/>
-      <c r="M18" s="142"/>
-      <c r="N18" s="142"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="110"/>
+      <c r="K18" s="110"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="110"/>
+      <c r="N18" s="110"/>
     </row>
     <row r="19" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G19" s="141"/>
-      <c r="H19" s="143"/>
-      <c r="I19" s="143"/>
-      <c r="J19" s="143"/>
-      <c r="K19" s="143"/>
-      <c r="L19" s="143"/>
-      <c r="M19" s="143"/>
-      <c r="N19" s="143"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G20" s="141"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="143"/>
-      <c r="J20" s="143"/>
-      <c r="K20" s="143"/>
-      <c r="L20" s="143"/>
-      <c r="M20" s="143"/>
-      <c r="N20" s="143"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="7:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="G21" s="141"/>
-      <c r="H21" s="142"/>
-      <c r="I21" s="142"/>
-      <c r="J21" s="142"/>
-      <c r="K21" s="142"/>
-      <c r="L21" s="142"/>
-      <c r="M21" s="142"/>
-      <c r="N21" s="142"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="110"/>
+      <c r="K21" s="110"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="110"/>
+      <c r="N21" s="110"/>
     </row>
     <row r="22" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G22" s="141"/>
-      <c r="H22" s="143"/>
-      <c r="I22" s="143"/>
-      <c r="J22" s="143"/>
-      <c r="K22" s="144"/>
-      <c r="L22" s="144"/>
-      <c r="M22" s="144"/>
-      <c r="N22" s="144"/>
-    </row>
-    <row r="23" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G23" s="143"/>
-      <c r="H23" s="143"/>
-      <c r="I23" s="143"/>
-      <c r="J23" s="143"/>
-      <c r="K23" s="143"/>
-      <c r="L23" s="143"/>
-      <c r="M23" s="143"/>
-      <c r="N23" s="143"/>
+      <c r="G22" s="33"/>
+      <c r="K22" s="111"/>
+      <c r="L22" s="111"/>
+      <c r="M22" s="111"/>
+      <c r="N22" s="111"/>
     </row>
     <row r="24" spans="7:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="G24" s="141"/>
-      <c r="H24" s="142"/>
-      <c r="I24" s="142"/>
-      <c r="J24" s="142"/>
-      <c r="K24" s="142"/>
-      <c r="L24" s="142"/>
-      <c r="M24" s="142"/>
-      <c r="N24" s="142"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="110"/>
+      <c r="I24" s="110"/>
+      <c r="J24" s="110"/>
+      <c r="K24" s="110"/>
+      <c r="L24" s="110"/>
+      <c r="M24" s="110"/>
+      <c r="N24" s="110"/>
     </row>
     <row r="25" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G25" s="141"/>
-      <c r="H25" s="145"/>
-      <c r="I25" s="145"/>
-      <c r="J25" s="145"/>
-      <c r="K25" s="145"/>
-      <c r="L25" s="145"/>
-      <c r="M25" s="146"/>
-      <c r="N25" s="143"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="143"/>
+      <c r="I25" s="143"/>
+      <c r="J25" s="143"/>
+      <c r="K25" s="143"/>
+      <c r="L25" s="143"/>
+      <c r="M25" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7248,10 +7226,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2049C0E-0B3A-41CB-95CB-257CB110AC6A}">
-  <dimension ref="A1:AM35"/>
+  <dimension ref="A1:AM34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7268,1750 +7246,1718 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="105" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="105" t="s">
         <v>409</v>
       </c>
-      <c r="C1" s="131" t="s">
+      <c r="C1" s="105" t="s">
         <v>346</v>
       </c>
-      <c r="D1" s="131" t="s">
+      <c r="D1" s="105" t="s">
         <v>410</v>
       </c>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
-      <c r="M1" s="131"/>
-      <c r="N1" s="131"/>
-      <c r="O1" s="131"/>
-      <c r="P1" s="131"/>
-      <c r="Q1" s="131"/>
-      <c r="R1" s="131"/>
-      <c r="S1" s="131"/>
-      <c r="T1" s="131"/>
-      <c r="U1" s="131"/>
-      <c r="V1" s="131"/>
-      <c r="W1" s="131"/>
-      <c r="X1" s="131"/>
-      <c r="Y1" s="131"/>
-      <c r="Z1" s="131"/>
-      <c r="AA1" s="131"/>
-      <c r="AB1" s="131"/>
-      <c r="AC1" s="131"/>
-      <c r="AD1" s="131"/>
-      <c r="AE1" s="131"/>
-      <c r="AF1" s="131"/>
-      <c r="AG1" s="131"/>
-      <c r="AH1" s="131"/>
-      <c r="AI1" s="131"/>
-      <c r="AJ1" s="131"/>
-      <c r="AK1" s="131"/>
-      <c r="AL1" s="131"/>
-      <c r="AM1" s="131"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="105"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="105"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="105"/>
+      <c r="AG1" s="105"/>
+      <c r="AH1" s="105"/>
+      <c r="AI1" s="105"/>
+      <c r="AJ1" s="105"/>
+      <c r="AK1" s="105"/>
+      <c r="AL1" s="105"/>
+      <c r="AM1" s="105"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="157" t="s">
         <v>347</v>
       </c>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="157" t="s">
         <v>348</v>
       </c>
-      <c r="C2" s="132" t="s">
+      <c r="C2" s="157" t="s">
         <v>349</v>
       </c>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="147" t="s">
+      <c r="D2" s="157"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="154" t="s">
         <v>350</v>
       </c>
-      <c r="G2" s="147" t="s">
+      <c r="G2" s="154" t="s">
         <v>351</v>
       </c>
-      <c r="H2" s="134" t="s">
+      <c r="H2" s="151" t="s">
         <v>417</v>
       </c>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134" t="s">
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="151" t="s">
         <v>418</v>
       </c>
-      <c r="M2" s="135"/>
-      <c r="N2" s="135"/>
-      <c r="O2" s="136"/>
-      <c r="P2" s="134" t="s">
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="151" t="s">
         <v>419</v>
       </c>
-      <c r="Q2" s="135"/>
-      <c r="R2" s="135"/>
-      <c r="S2" s="136"/>
-      <c r="T2" s="134" t="s">
+      <c r="Q2" s="152"/>
+      <c r="R2" s="152"/>
+      <c r="S2" s="153"/>
+      <c r="T2" s="151" t="s">
         <v>358</v>
       </c>
-      <c r="U2" s="135"/>
-      <c r="V2" s="135"/>
-      <c r="W2" s="136"/>
-      <c r="X2" s="134" t="s">
+      <c r="U2" s="152"/>
+      <c r="V2" s="152"/>
+      <c r="W2" s="153"/>
+      <c r="X2" s="151" t="s">
         <v>359</v>
       </c>
-      <c r="Y2" s="135"/>
-      <c r="Z2" s="135"/>
-      <c r="AA2" s="136"/>
-      <c r="AB2" s="134" t="s">
+      <c r="Y2" s="152"/>
+      <c r="Z2" s="152"/>
+      <c r="AA2" s="153"/>
+      <c r="AB2" s="151" t="s">
         <v>360</v>
       </c>
-      <c r="AC2" s="135"/>
-      <c r="AD2" s="135"/>
-      <c r="AE2" s="136"/>
-      <c r="AF2" s="134" t="s">
+      <c r="AC2" s="152"/>
+      <c r="AD2" s="152"/>
+      <c r="AE2" s="153"/>
+      <c r="AF2" s="151" t="s">
         <v>361</v>
       </c>
-      <c r="AG2" s="135"/>
-      <c r="AH2" s="135"/>
-      <c r="AI2" s="136"/>
-      <c r="AJ2" s="134" t="s">
+      <c r="AG2" s="152"/>
+      <c r="AH2" s="152"/>
+      <c r="AI2" s="153"/>
+      <c r="AJ2" s="151" t="s">
         <v>362</v>
       </c>
-      <c r="AK2" s="135"/>
-      <c r="AL2" s="135"/>
-      <c r="AM2" s="136"/>
+      <c r="AK2" s="152"/>
+      <c r="AL2" s="152"/>
+      <c r="AM2" s="153"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="132"/>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="131">
+      <c r="A3" s="157"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="156"/>
+      <c r="H3" s="105">
         <v>1</v>
       </c>
-      <c r="I3" s="131">
+      <c r="I3" s="105">
         <v>2</v>
       </c>
-      <c r="J3" s="131">
+      <c r="J3" s="105">
         <v>3</v>
       </c>
-      <c r="K3" s="131">
+      <c r="K3" s="105">
         <v>4</v>
       </c>
-      <c r="L3" s="131">
+      <c r="L3" s="105">
         <v>1</v>
       </c>
-      <c r="M3" s="131">
+      <c r="M3" s="105">
         <v>2</v>
       </c>
-      <c r="N3" s="131">
+      <c r="N3" s="105">
         <v>3</v>
       </c>
-      <c r="O3" s="131">
+      <c r="O3" s="105">
         <v>4</v>
       </c>
-      <c r="P3" s="131">
+      <c r="P3" s="105">
         <v>1</v>
       </c>
-      <c r="Q3" s="131">
+      <c r="Q3" s="105">
         <v>2</v>
       </c>
-      <c r="R3" s="131">
+      <c r="R3" s="105">
         <v>3</v>
       </c>
-      <c r="S3" s="131">
+      <c r="S3" s="105">
         <v>4</v>
       </c>
-      <c r="T3" s="131">
+      <c r="T3" s="105">
         <v>1</v>
       </c>
-      <c r="U3" s="131">
+      <c r="U3" s="105">
         <v>2</v>
       </c>
-      <c r="V3" s="131">
+      <c r="V3" s="105">
         <v>3</v>
       </c>
-      <c r="W3" s="131">
+      <c r="W3" s="105">
         <v>4</v>
       </c>
-      <c r="X3" s="131">
+      <c r="X3" s="105">
         <v>1</v>
       </c>
-      <c r="Y3" s="131">
+      <c r="Y3" s="105">
         <v>2</v>
       </c>
-      <c r="Z3" s="131">
+      <c r="Z3" s="105">
         <v>3</v>
       </c>
-      <c r="AA3" s="131">
+      <c r="AA3" s="105">
         <v>4</v>
       </c>
-      <c r="AB3" s="131">
+      <c r="AB3" s="105">
         <v>1</v>
       </c>
-      <c r="AC3" s="131">
+      <c r="AC3" s="105">
         <v>2</v>
       </c>
-      <c r="AD3" s="131">
+      <c r="AD3" s="105">
         <v>3</v>
       </c>
-      <c r="AE3" s="131">
+      <c r="AE3" s="105">
         <v>4</v>
       </c>
-      <c r="AF3" s="131">
+      <c r="AF3" s="105">
         <v>1</v>
       </c>
-      <c r="AG3" s="131">
+      <c r="AG3" s="105">
         <v>2</v>
       </c>
-      <c r="AH3" s="131">
+      <c r="AH3" s="105">
         <v>3</v>
       </c>
-      <c r="AI3" s="131">
+      <c r="AI3" s="105">
         <v>4</v>
       </c>
-      <c r="AJ3" s="131">
+      <c r="AJ3" s="105">
         <v>1</v>
       </c>
-      <c r="AK3" s="131">
+      <c r="AK3" s="105">
         <v>2</v>
       </c>
-      <c r="AL3" s="131">
+      <c r="AL3" s="105">
         <v>3</v>
       </c>
-      <c r="AM3" s="131">
+      <c r="AM3" s="105">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="105" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="105" t="s">
         <v>363</v>
       </c>
-      <c r="C4" s="131" t="s">
+      <c r="C4" s="105" t="s">
         <v>363</v>
       </c>
-      <c r="D4" s="131"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131" t="s">
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105" t="s">
         <v>413</v>
       </c>
-      <c r="G4" s="131" t="s">
+      <c r="G4" s="105" t="s">
         <v>415</v>
       </c>
-      <c r="H4" s="131"/>
-      <c r="I4" s="131"/>
-      <c r="J4" s="137"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131"/>
-      <c r="N4" s="131"/>
-      <c r="O4" s="131"/>
-      <c r="P4" s="131"/>
-      <c r="Q4" s="131"/>
-      <c r="R4" s="131"/>
-      <c r="S4" s="131"/>
-      <c r="T4" s="131"/>
-      <c r="U4" s="131"/>
-      <c r="V4" s="131"/>
-      <c r="W4" s="131"/>
-      <c r="X4" s="131"/>
-      <c r="Y4" s="131"/>
-      <c r="Z4" s="131"/>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="131"/>
-      <c r="AC4" s="131"/>
-      <c r="AD4" s="131"/>
-      <c r="AE4" s="131"/>
-      <c r="AF4" s="131"/>
-      <c r="AG4" s="131"/>
-      <c r="AH4" s="131"/>
-      <c r="AI4" s="131"/>
-      <c r="AJ4" s="131"/>
-      <c r="AK4" s="131"/>
-      <c r="AL4" s="131"/>
-      <c r="AM4" s="131"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
+      <c r="O4" s="105"/>
+      <c r="P4" s="105"/>
+      <c r="Q4" s="105"/>
+      <c r="R4" s="105"/>
+      <c r="S4" s="105"/>
+      <c r="T4" s="105"/>
+      <c r="U4" s="105"/>
+      <c r="V4" s="105"/>
+      <c r="W4" s="105"/>
+      <c r="X4" s="105"/>
+      <c r="Y4" s="105"/>
+      <c r="Z4" s="105"/>
+      <c r="AA4" s="105"/>
+      <c r="AB4" s="105"/>
+      <c r="AC4" s="105"/>
+      <c r="AD4" s="105"/>
+      <c r="AE4" s="105"/>
+      <c r="AF4" s="105"/>
+      <c r="AG4" s="105"/>
+      <c r="AH4" s="105"/>
+      <c r="AI4" s="105"/>
+      <c r="AJ4" s="105"/>
+      <c r="AK4" s="105"/>
+      <c r="AL4" s="105"/>
+      <c r="AM4" s="105"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A5" s="131" t="s">
+      <c r="A5" s="105" t="s">
         <v>353</v>
       </c>
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="105" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="105" t="s">
         <v>364</v>
       </c>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131" t="s">
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105" t="s">
         <v>416</v>
       </c>
-      <c r="G5" s="131" t="s">
+      <c r="G5" s="105" t="s">
         <v>414</v>
       </c>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="137"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
-      <c r="N5" s="131"/>
-      <c r="O5" s="131"/>
-      <c r="P5" s="131"/>
-      <c r="Q5" s="131"/>
-      <c r="R5" s="131"/>
-      <c r="S5" s="131"/>
-      <c r="T5" s="131"/>
-      <c r="U5" s="131"/>
-      <c r="V5" s="131"/>
-      <c r="W5" s="131"/>
-      <c r="X5" s="131"/>
-      <c r="Y5" s="131"/>
-      <c r="Z5" s="131"/>
-      <c r="AA5" s="131"/>
-      <c r="AB5" s="131"/>
-      <c r="AC5" s="131"/>
-      <c r="AD5" s="131"/>
-      <c r="AE5" s="131"/>
-      <c r="AF5" s="131"/>
-      <c r="AG5" s="131"/>
-      <c r="AH5" s="131"/>
-      <c r="AI5" s="131"/>
-      <c r="AJ5" s="131"/>
-      <c r="AK5" s="131"/>
-      <c r="AL5" s="131"/>
-      <c r="AM5" s="131"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="105"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="105"/>
+      <c r="Q5" s="105"/>
+      <c r="R5" s="105"/>
+      <c r="S5" s="105"/>
+      <c r="T5" s="105"/>
+      <c r="U5" s="105"/>
+      <c r="V5" s="105"/>
+      <c r="W5" s="105"/>
+      <c r="X5" s="105"/>
+      <c r="Y5" s="105"/>
+      <c r="Z5" s="105"/>
+      <c r="AA5" s="105"/>
+      <c r="AB5" s="105"/>
+      <c r="AC5" s="105"/>
+      <c r="AD5" s="105"/>
+      <c r="AE5" s="105"/>
+      <c r="AF5" s="105"/>
+      <c r="AG5" s="105"/>
+      <c r="AH5" s="105"/>
+      <c r="AI5" s="105"/>
+      <c r="AJ5" s="105"/>
+      <c r="AK5" s="105"/>
+      <c r="AL5" s="105"/>
+      <c r="AM5" s="105"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="132" t="s">
+      <c r="A6" s="157" t="s">
         <v>354</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="105" t="s">
         <v>366</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131" t="s">
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105" t="s">
         <v>411</v>
       </c>
-      <c r="G6" s="131" t="s">
+      <c r="G6" s="105" t="s">
         <v>412</v>
       </c>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="137"/>
-      <c r="M6" s="137"/>
-      <c r="N6" s="131"/>
-      <c r="O6" s="131"/>
-      <c r="P6" s="131"/>
-      <c r="Q6" s="131"/>
-      <c r="R6" s="131"/>
-      <c r="S6" s="131"/>
-      <c r="T6" s="131"/>
-      <c r="U6" s="131"/>
-      <c r="V6" s="131"/>
-      <c r="W6" s="131"/>
-      <c r="X6" s="131"/>
-      <c r="Y6" s="131"/>
-      <c r="Z6" s="131"/>
-      <c r="AA6" s="131"/>
-      <c r="AB6" s="131"/>
-      <c r="AC6" s="131"/>
-      <c r="AD6" s="131"/>
-      <c r="AE6" s="131"/>
-      <c r="AF6" s="131"/>
-      <c r="AG6" s="131"/>
-      <c r="AH6" s="131"/>
-      <c r="AI6" s="131"/>
-      <c r="AJ6" s="131"/>
-      <c r="AK6" s="131"/>
-      <c r="AL6" s="131"/>
-      <c r="AM6" s="131"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="105"/>
+      <c r="P6" s="105"/>
+      <c r="Q6" s="105"/>
+      <c r="R6" s="105"/>
+      <c r="S6" s="105"/>
+      <c r="T6" s="105"/>
+      <c r="U6" s="105"/>
+      <c r="V6" s="105"/>
+      <c r="W6" s="105"/>
+      <c r="X6" s="105"/>
+      <c r="Y6" s="105"/>
+      <c r="Z6" s="105"/>
+      <c r="AA6" s="105"/>
+      <c r="AB6" s="105"/>
+      <c r="AC6" s="105"/>
+      <c r="AD6" s="105"/>
+      <c r="AE6" s="105"/>
+      <c r="AF6" s="105"/>
+      <c r="AG6" s="105"/>
+      <c r="AH6" s="105"/>
+      <c r="AI6" s="105"/>
+      <c r="AJ6" s="105"/>
+      <c r="AK6" s="105"/>
+      <c r="AL6" s="105"/>
+      <c r="AM6" s="105"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="132"/>
-      <c r="B7" s="131" t="s">
+      <c r="A7" s="157"/>
+      <c r="B7" s="105" t="s">
         <v>367</v>
       </c>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="131"/>
-      <c r="F7" s="131" t="s">
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105" t="s">
         <v>411</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="105" t="s">
         <v>412</v>
       </c>
-      <c r="H7" s="131"/>
-      <c r="I7" s="131"/>
-      <c r="J7" s="131"/>
-      <c r="K7" s="131"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="137"/>
-      <c r="N7" s="131"/>
-      <c r="O7" s="131"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="131"/>
-      <c r="R7" s="131"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="131"/>
-      <c r="U7" s="131"/>
-      <c r="V7" s="131"/>
-      <c r="W7" s="131"/>
-      <c r="X7" s="131"/>
-      <c r="Y7" s="131"/>
-      <c r="Z7" s="131"/>
-      <c r="AA7" s="131"/>
-      <c r="AB7" s="131"/>
-      <c r="AC7" s="131"/>
-      <c r="AD7" s="131"/>
-      <c r="AE7" s="131"/>
-      <c r="AF7" s="131"/>
-      <c r="AG7" s="131"/>
-      <c r="AH7" s="131"/>
-      <c r="AI7" s="131"/>
-      <c r="AJ7" s="131"/>
-      <c r="AK7" s="131"/>
-      <c r="AL7" s="131"/>
-      <c r="AM7" s="131"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="105"/>
+      <c r="O7" s="105"/>
+      <c r="P7" s="105"/>
+      <c r="Q7" s="105"/>
+      <c r="R7" s="105"/>
+      <c r="S7" s="105"/>
+      <c r="T7" s="105"/>
+      <c r="U7" s="105"/>
+      <c r="V7" s="105"/>
+      <c r="W7" s="105"/>
+      <c r="X7" s="105"/>
+      <c r="Y7" s="105"/>
+      <c r="Z7" s="105"/>
+      <c r="AA7" s="105"/>
+      <c r="AB7" s="105"/>
+      <c r="AC7" s="105"/>
+      <c r="AD7" s="105"/>
+      <c r="AE7" s="105"/>
+      <c r="AF7" s="105"/>
+      <c r="AG7" s="105"/>
+      <c r="AH7" s="105"/>
+      <c r="AI7" s="105"/>
+      <c r="AJ7" s="105"/>
+      <c r="AK7" s="105"/>
+      <c r="AL7" s="105"/>
+      <c r="AM7" s="105"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="147" t="s">
+      <c r="A8" s="154" t="s">
         <v>355</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="105" t="s">
         <v>368</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="105" t="s">
         <v>368</v>
       </c>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131" t="s">
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105" t="s">
         <v>420</v>
       </c>
-      <c r="G8" s="131" t="s">
+      <c r="G8" s="105" t="s">
         <v>409</v>
       </c>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="131"/>
-      <c r="L8" s="131"/>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="137"/>
-      <c r="S8" s="137"/>
-      <c r="T8" s="137"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
-      <c r="AB8" s="131"/>
-      <c r="AC8" s="131"/>
-      <c r="AD8" s="131"/>
-      <c r="AE8" s="131"/>
-      <c r="AF8" s="131"/>
-      <c r="AG8" s="131"/>
-      <c r="AH8" s="131"/>
-      <c r="AI8" s="131"/>
-      <c r="AJ8" s="131"/>
-      <c r="AK8" s="131"/>
-      <c r="AL8" s="131"/>
-      <c r="AM8" s="131"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="105"/>
+      <c r="O8" s="105"/>
+      <c r="P8" s="105"/>
+      <c r="Q8" s="105"/>
+      <c r="R8" s="107"/>
+      <c r="S8" s="107"/>
+      <c r="T8" s="107"/>
+      <c r="U8" s="105"/>
+      <c r="V8" s="105"/>
+      <c r="W8" s="105"/>
+      <c r="X8" s="105"/>
+      <c r="Y8" s="105"/>
+      <c r="Z8" s="105"/>
+      <c r="AA8" s="105"/>
+      <c r="AB8" s="105"/>
+      <c r="AC8" s="105"/>
+      <c r="AD8" s="105"/>
+      <c r="AE8" s="105"/>
+      <c r="AF8" s="105"/>
+      <c r="AG8" s="105"/>
+      <c r="AH8" s="105"/>
+      <c r="AI8" s="105"/>
+      <c r="AJ8" s="105"/>
+      <c r="AK8" s="105"/>
+      <c r="AL8" s="105"/>
+      <c r="AM8" s="105"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="148"/>
-      <c r="B9" s="132" t="s">
+      <c r="A9" s="155"/>
+      <c r="B9" s="157" t="s">
         <v>355</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="157" t="s">
         <v>386</v>
       </c>
-      <c r="D9" s="131" t="s">
+      <c r="D9" s="105" t="s">
         <v>387</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131" t="s">
+      <c r="E9" s="105"/>
+      <c r="F9" s="105" t="s">
         <v>396</v>
       </c>
-      <c r="G9" s="131" t="s">
+      <c r="G9" s="105" t="s">
         <v>397</v>
       </c>
-      <c r="H9" s="131"/>
-      <c r="I9" s="131"/>
-      <c r="J9" s="131"/>
-      <c r="K9" s="131"/>
-      <c r="L9" s="131"/>
-      <c r="M9" s="131"/>
-      <c r="N9" s="131"/>
-      <c r="O9" s="131"/>
-      <c r="P9" s="131"/>
-      <c r="Q9" s="131"/>
-      <c r="R9" s="131"/>
-      <c r="S9" s="131"/>
-      <c r="T9" s="131"/>
-      <c r="U9" s="131"/>
-      <c r="V9" s="131"/>
-      <c r="W9" s="131"/>
-      <c r="X9" s="137"/>
-      <c r="Y9" s="131"/>
-      <c r="Z9" s="131"/>
-      <c r="AA9" s="131"/>
-      <c r="AB9" s="131"/>
-      <c r="AC9" s="131"/>
-      <c r="AD9" s="131"/>
-      <c r="AE9" s="131"/>
-      <c r="AF9" s="131"/>
-      <c r="AG9" s="131"/>
-      <c r="AH9" s="131"/>
-      <c r="AI9" s="131"/>
-      <c r="AJ9" s="131"/>
-      <c r="AK9" s="131"/>
-      <c r="AL9" s="131"/>
-      <c r="AM9" s="131"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="105"/>
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
+      <c r="S9" s="105"/>
+      <c r="T9" s="105"/>
+      <c r="U9" s="105"/>
+      <c r="V9" s="105"/>
+      <c r="W9" s="105"/>
+      <c r="X9" s="107"/>
+      <c r="Y9" s="105"/>
+      <c r="Z9" s="105"/>
+      <c r="AA9" s="105"/>
+      <c r="AB9" s="105"/>
+      <c r="AC9" s="105"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="105"/>
+      <c r="AG9" s="105"/>
+      <c r="AH9" s="105"/>
+      <c r="AI9" s="105"/>
+      <c r="AJ9" s="105"/>
+      <c r="AK9" s="105"/>
+      <c r="AL9" s="105"/>
+      <c r="AM9" s="105"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="148"/>
-      <c r="B10" s="132"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="131" t="s">
+      <c r="A10" s="155"/>
+      <c r="B10" s="157"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="105" t="s">
         <v>390</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131" t="s">
+      <c r="E10" s="105"/>
+      <c r="F10" s="105" t="s">
         <v>396</v>
       </c>
-      <c r="G10" s="131" t="s">
+      <c r="G10" s="105" t="s">
         <v>397</v>
       </c>
-      <c r="H10" s="131"/>
-      <c r="I10" s="131"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="131"/>
-      <c r="L10" s="131"/>
-      <c r="M10" s="131"/>
-      <c r="N10" s="131"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="131"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="131"/>
-      <c r="T10" s="131"/>
-      <c r="U10" s="131"/>
-      <c r="V10" s="131"/>
-      <c r="W10" s="131"/>
-      <c r="X10" s="137"/>
-      <c r="Y10" s="131"/>
-      <c r="Z10" s="131"/>
-      <c r="AA10" s="131"/>
-      <c r="AB10" s="131"/>
-      <c r="AC10" s="131"/>
-      <c r="AD10" s="131"/>
-      <c r="AE10" s="131"/>
-      <c r="AF10" s="131"/>
-      <c r="AG10" s="131"/>
-      <c r="AH10" s="131"/>
-      <c r="AI10" s="131"/>
-      <c r="AJ10" s="131"/>
-      <c r="AK10" s="131"/>
-      <c r="AL10" s="131"/>
-      <c r="AM10" s="131"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="105"/>
+      <c r="N10" s="105"/>
+      <c r="O10" s="105"/>
+      <c r="P10" s="105"/>
+      <c r="Q10" s="105"/>
+      <c r="R10" s="105"/>
+      <c r="S10" s="105"/>
+      <c r="T10" s="105"/>
+      <c r="U10" s="105"/>
+      <c r="V10" s="105"/>
+      <c r="W10" s="105"/>
+      <c r="X10" s="107"/>
+      <c r="Y10" s="105"/>
+      <c r="Z10" s="105"/>
+      <c r="AA10" s="105"/>
+      <c r="AB10" s="105"/>
+      <c r="AC10" s="105"/>
+      <c r="AD10" s="105"/>
+      <c r="AE10" s="105"/>
+      <c r="AF10" s="105"/>
+      <c r="AG10" s="105"/>
+      <c r="AH10" s="105"/>
+      <c r="AI10" s="105"/>
+      <c r="AJ10" s="105"/>
+      <c r="AK10" s="105"/>
+      <c r="AL10" s="105"/>
+      <c r="AM10" s="105"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A11" s="148"/>
-      <c r="B11" s="132"/>
-      <c r="C11" s="132" t="s">
+      <c r="A11" s="155"/>
+      <c r="B11" s="157"/>
+      <c r="C11" s="157" t="s">
         <v>370</v>
       </c>
-      <c r="D11" s="131" t="s">
+      <c r="D11" s="105" t="s">
         <v>371</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="131" t="s">
+      <c r="E11" s="105"/>
+      <c r="F11" s="105" t="s">
         <v>398</v>
       </c>
-      <c r="G11" s="131" t="s">
+      <c r="G11" s="105" t="s">
         <v>399</v>
       </c>
-      <c r="H11" s="131"/>
-      <c r="I11" s="131"/>
-      <c r="J11" s="131"/>
-      <c r="K11" s="131"/>
-      <c r="L11" s="131"/>
-      <c r="M11" s="131"/>
-      <c r="N11" s="131"/>
-      <c r="O11" s="131"/>
-      <c r="P11" s="131"/>
-      <c r="Q11" s="131"/>
-      <c r="R11" s="131"/>
-      <c r="S11" s="131"/>
-      <c r="T11" s="131"/>
-      <c r="U11" s="131"/>
-      <c r="V11" s="131"/>
-      <c r="W11" s="131"/>
-      <c r="X11" s="131"/>
-      <c r="Y11" s="137"/>
-      <c r="Z11" s="137"/>
-      <c r="AA11" s="137"/>
-      <c r="AB11" s="131"/>
-      <c r="AC11" s="131"/>
-      <c r="AD11" s="131"/>
-      <c r="AE11" s="131"/>
-      <c r="AF11" s="131"/>
-      <c r="AG11" s="131"/>
-      <c r="AH11" s="131"/>
-      <c r="AI11" s="131"/>
-      <c r="AJ11" s="131"/>
-      <c r="AK11" s="131"/>
-      <c r="AL11" s="131"/>
-      <c r="AM11" s="131"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="105"/>
+      <c r="N11" s="105"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="105"/>
+      <c r="Q11" s="105"/>
+      <c r="R11" s="105"/>
+      <c r="S11" s="105"/>
+      <c r="T11" s="105"/>
+      <c r="U11" s="105"/>
+      <c r="V11" s="105"/>
+      <c r="W11" s="105"/>
+      <c r="X11" s="105"/>
+      <c r="Y11" s="107"/>
+      <c r="Z11" s="107"/>
+      <c r="AA11" s="107"/>
+      <c r="AB11" s="105"/>
+      <c r="AC11" s="105"/>
+      <c r="AD11" s="105"/>
+      <c r="AE11" s="105"/>
+      <c r="AF11" s="105"/>
+      <c r="AG11" s="105"/>
+      <c r="AH11" s="105"/>
+      <c r="AI11" s="105"/>
+      <c r="AJ11" s="105"/>
+      <c r="AK11" s="105"/>
+      <c r="AL11" s="105"/>
+      <c r="AM11" s="105"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="148"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="131" t="s">
+      <c r="A12" s="155"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="157"/>
+      <c r="D12" s="105" t="s">
         <v>372</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131" t="s">
+      <c r="E12" s="105"/>
+      <c r="F12" s="105" t="s">
         <v>400</v>
       </c>
-      <c r="G12" s="131" t="s">
+      <c r="G12" s="105" t="s">
         <v>421</v>
       </c>
-      <c r="H12" s="131"/>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="131"/>
-      <c r="M12" s="131"/>
-      <c r="N12" s="131"/>
-      <c r="O12" s="131"/>
-      <c r="P12" s="131"/>
-      <c r="Q12" s="131"/>
-      <c r="R12" s="131"/>
-      <c r="S12" s="131"/>
-      <c r="T12" s="131"/>
-      <c r="U12" s="131"/>
-      <c r="V12" s="131"/>
-      <c r="W12" s="131"/>
-      <c r="X12" s="131"/>
-      <c r="Y12" s="131"/>
-      <c r="Z12" s="131"/>
-      <c r="AA12" s="137"/>
-      <c r="AB12" s="137"/>
-      <c r="AC12" s="131"/>
-      <c r="AD12" s="131"/>
-      <c r="AE12" s="131"/>
-      <c r="AF12" s="131"/>
-      <c r="AG12" s="131"/>
-      <c r="AH12" s="131"/>
-      <c r="AI12" s="131"/>
-      <c r="AJ12" s="131"/>
-      <c r="AK12" s="131"/>
-      <c r="AL12" s="131"/>
-      <c r="AM12" s="131"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="105"/>
+      <c r="N12" s="105"/>
+      <c r="O12" s="105"/>
+      <c r="P12" s="105"/>
+      <c r="Q12" s="105"/>
+      <c r="R12" s="105"/>
+      <c r="S12" s="105"/>
+      <c r="T12" s="105"/>
+      <c r="U12" s="105"/>
+      <c r="V12" s="105"/>
+      <c r="W12" s="105"/>
+      <c r="X12" s="105"/>
+      <c r="Y12" s="105"/>
+      <c r="Z12" s="105"/>
+      <c r="AA12" s="107"/>
+      <c r="AB12" s="107"/>
+      <c r="AC12" s="105"/>
+      <c r="AD12" s="105"/>
+      <c r="AE12" s="105"/>
+      <c r="AF12" s="105"/>
+      <c r="AG12" s="105"/>
+      <c r="AH12" s="105"/>
+      <c r="AI12" s="105"/>
+      <c r="AJ12" s="105"/>
+      <c r="AK12" s="105"/>
+      <c r="AL12" s="105"/>
+      <c r="AM12" s="105"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A13" s="148"/>
-      <c r="B13" s="132"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="131" t="s">
+      <c r="A13" s="155"/>
+      <c r="B13" s="157"/>
+      <c r="C13" s="157"/>
+      <c r="D13" s="105" t="s">
         <v>373</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="131" t="s">
+      <c r="E13" s="105"/>
+      <c r="F13" s="105" t="s">
         <v>401</v>
       </c>
-      <c r="G13" s="131" t="s">
+      <c r="G13" s="105" t="s">
         <v>402</v>
       </c>
-      <c r="H13" s="131"/>
-      <c r="I13" s="131"/>
-      <c r="J13" s="131"/>
-      <c r="K13" s="131"/>
-      <c r="L13" s="131"/>
-      <c r="M13" s="131"/>
-      <c r="N13" s="131"/>
-      <c r="O13" s="131"/>
-      <c r="P13" s="131"/>
-      <c r="Q13" s="131"/>
-      <c r="R13" s="131"/>
-      <c r="S13" s="131"/>
-      <c r="T13" s="131"/>
-      <c r="U13" s="131"/>
-      <c r="V13" s="131"/>
-      <c r="W13" s="131"/>
-      <c r="X13" s="131"/>
-      <c r="Y13" s="131"/>
-      <c r="Z13" s="131"/>
-      <c r="AA13" s="131"/>
-      <c r="AB13" s="131"/>
-      <c r="AC13" s="131"/>
-      <c r="AD13" s="137"/>
-      <c r="AE13" s="137"/>
-      <c r="AF13" s="131"/>
-      <c r="AG13" s="131"/>
-      <c r="AH13" s="131"/>
-      <c r="AI13" s="131"/>
-      <c r="AJ13" s="131"/>
-      <c r="AK13" s="131"/>
-      <c r="AL13" s="131"/>
-      <c r="AM13" s="131"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
+      <c r="N13" s="105"/>
+      <c r="O13" s="105"/>
+      <c r="P13" s="105"/>
+      <c r="Q13" s="105"/>
+      <c r="R13" s="105"/>
+      <c r="S13" s="105"/>
+      <c r="T13" s="105"/>
+      <c r="U13" s="105"/>
+      <c r="V13" s="105"/>
+      <c r="W13" s="105"/>
+      <c r="X13" s="105"/>
+      <c r="Y13" s="105"/>
+      <c r="Z13" s="105"/>
+      <c r="AA13" s="105"/>
+      <c r="AB13" s="105"/>
+      <c r="AC13" s="105"/>
+      <c r="AD13" s="107"/>
+      <c r="AE13" s="107"/>
+      <c r="AF13" s="105"/>
+      <c r="AG13" s="105"/>
+      <c r="AH13" s="105"/>
+      <c r="AI13" s="105"/>
+      <c r="AJ13" s="105"/>
+      <c r="AK13" s="105"/>
+      <c r="AL13" s="105"/>
+      <c r="AM13" s="105"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="148"/>
-      <c r="B14" s="132"/>
-      <c r="C14" s="132"/>
-      <c r="D14" s="132" t="s">
+      <c r="A14" s="155"/>
+      <c r="B14" s="157"/>
+      <c r="C14" s="157"/>
+      <c r="D14" s="157" t="s">
         <v>374</v>
       </c>
-      <c r="E14" s="131" t="s">
+      <c r="E14" s="105" t="s">
         <v>376</v>
       </c>
-      <c r="F14" s="131" t="s">
+      <c r="F14" s="105" t="s">
         <v>404</v>
       </c>
-      <c r="G14" s="131" t="s">
+      <c r="G14" s="105" t="s">
         <v>405</v>
       </c>
-      <c r="H14" s="131"/>
-      <c r="I14" s="131"/>
-      <c r="J14" s="131"/>
-      <c r="K14" s="131"/>
-      <c r="L14" s="131"/>
-      <c r="M14" s="131"/>
-      <c r="N14" s="131"/>
-      <c r="O14" s="131"/>
-      <c r="P14" s="131"/>
-      <c r="Q14" s="131"/>
-      <c r="R14" s="131"/>
-      <c r="S14" s="131"/>
-      <c r="T14" s="131"/>
-      <c r="U14" s="131"/>
-      <c r="V14" s="131"/>
-      <c r="W14" s="131"/>
-      <c r="X14" s="131"/>
-      <c r="Y14" s="131"/>
-      <c r="Z14" s="131"/>
-      <c r="AA14" s="131"/>
-      <c r="AB14" s="131"/>
-      <c r="AC14" s="131"/>
-      <c r="AD14" s="131"/>
-      <c r="AE14" s="137"/>
-      <c r="AF14" s="131"/>
-      <c r="AG14" s="131"/>
-      <c r="AH14" s="131"/>
-      <c r="AI14" s="131"/>
-      <c r="AJ14" s="131"/>
-      <c r="AK14" s="131"/>
-      <c r="AL14" s="131"/>
-      <c r="AM14" s="131"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="105"/>
+      <c r="N14" s="105"/>
+      <c r="O14" s="105"/>
+      <c r="P14" s="105"/>
+      <c r="Q14" s="105"/>
+      <c r="R14" s="105"/>
+      <c r="S14" s="105"/>
+      <c r="T14" s="105"/>
+      <c r="U14" s="105"/>
+      <c r="V14" s="105"/>
+      <c r="W14" s="105"/>
+      <c r="X14" s="105"/>
+      <c r="Y14" s="105"/>
+      <c r="Z14" s="105"/>
+      <c r="AA14" s="105"/>
+      <c r="AB14" s="105"/>
+      <c r="AC14" s="105"/>
+      <c r="AD14" s="105"/>
+      <c r="AE14" s="107"/>
+      <c r="AF14" s="105"/>
+      <c r="AG14" s="105"/>
+      <c r="AH14" s="105"/>
+      <c r="AI14" s="105"/>
+      <c r="AJ14" s="105"/>
+      <c r="AK14" s="105"/>
+      <c r="AL14" s="105"/>
+      <c r="AM14" s="105"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A15" s="148"/>
-      <c r="B15" s="132"/>
-      <c r="C15" s="132"/>
-      <c r="D15" s="132"/>
-      <c r="E15" s="131" t="s">
+      <c r="A15" s="155"/>
+      <c r="B15" s="157"/>
+      <c r="C15" s="157"/>
+      <c r="D15" s="157"/>
+      <c r="E15" s="105" t="s">
         <v>375</v>
       </c>
-      <c r="F15" s="131" t="s">
+      <c r="F15" s="105" t="s">
         <v>404</v>
       </c>
-      <c r="G15" s="131" t="s">
+      <c r="G15" s="105" t="s">
         <v>405</v>
       </c>
-      <c r="H15" s="131"/>
-      <c r="I15" s="131"/>
-      <c r="J15" s="131"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="131"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="131"/>
-      <c r="O15" s="131"/>
-      <c r="P15" s="131"/>
-      <c r="Q15" s="131"/>
-      <c r="R15" s="131"/>
-      <c r="S15" s="131"/>
-      <c r="T15" s="131"/>
-      <c r="U15" s="131"/>
-      <c r="V15" s="131"/>
-      <c r="W15" s="131"/>
-      <c r="X15" s="131"/>
-      <c r="Y15" s="131"/>
-      <c r="Z15" s="131"/>
-      <c r="AA15" s="131"/>
-      <c r="AB15" s="131"/>
-      <c r="AC15" s="131"/>
-      <c r="AD15" s="131"/>
-      <c r="AE15" s="137"/>
-      <c r="AF15" s="131"/>
-      <c r="AG15" s="131"/>
-      <c r="AH15" s="131"/>
-      <c r="AI15" s="131"/>
-      <c r="AJ15" s="131"/>
-      <c r="AK15" s="131"/>
-      <c r="AL15" s="131"/>
-      <c r="AM15" s="131"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="105"/>
+      <c r="O15" s="105"/>
+      <c r="P15" s="105"/>
+      <c r="Q15" s="105"/>
+      <c r="R15" s="105"/>
+      <c r="S15" s="105"/>
+      <c r="T15" s="105"/>
+      <c r="U15" s="105"/>
+      <c r="V15" s="105"/>
+      <c r="W15" s="105"/>
+      <c r="X15" s="105"/>
+      <c r="Y15" s="105"/>
+      <c r="Z15" s="105"/>
+      <c r="AA15" s="105"/>
+      <c r="AB15" s="105"/>
+      <c r="AC15" s="105"/>
+      <c r="AD15" s="105"/>
+      <c r="AE15" s="107"/>
+      <c r="AF15" s="105"/>
+      <c r="AG15" s="105"/>
+      <c r="AH15" s="105"/>
+      <c r="AI15" s="105"/>
+      <c r="AJ15" s="105"/>
+      <c r="AK15" s="105"/>
+      <c r="AL15" s="105"/>
+      <c r="AM15" s="105"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="148"/>
-      <c r="B16" s="132"/>
-      <c r="C16" s="132" t="s">
+      <c r="A16" s="155"/>
+      <c r="B16" s="157"/>
+      <c r="C16" s="157" t="s">
         <v>377</v>
       </c>
-      <c r="D16" s="131" t="s">
+      <c r="D16" s="105" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131" t="s">
+      <c r="E16" s="105"/>
+      <c r="F16" s="105" t="s">
         <v>406</v>
       </c>
-      <c r="G16" s="131" t="s">
-        <v>422</v>
-      </c>
-      <c r="H16" s="131"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="131"/>
-      <c r="L16" s="131"/>
-      <c r="M16" s="131"/>
-      <c r="N16" s="131"/>
-      <c r="O16" s="131"/>
-      <c r="P16" s="131"/>
-      <c r="Q16" s="131"/>
-      <c r="R16" s="131"/>
-      <c r="S16" s="131"/>
-      <c r="T16" s="131"/>
-      <c r="U16" s="131"/>
-      <c r="V16" s="131"/>
-      <c r="W16" s="131"/>
-      <c r="X16" s="131"/>
-      <c r="Y16" s="131"/>
-      <c r="Z16" s="131"/>
-      <c r="AA16" s="131"/>
-      <c r="AB16" s="131"/>
-      <c r="AC16" s="131"/>
-      <c r="AD16" s="131"/>
-      <c r="AE16" s="131"/>
-      <c r="AF16" s="137"/>
-      <c r="AG16" s="131"/>
-      <c r="AH16" s="131"/>
-      <c r="AI16" s="131"/>
-      <c r="AJ16" s="131"/>
-      <c r="AK16" s="131"/>
-      <c r="AL16" s="131"/>
-      <c r="AM16" s="131"/>
+      <c r="G16" s="105" t="s">
+        <v>451</v>
+      </c>
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="105"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="105"/>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="105"/>
+      <c r="S16" s="105"/>
+      <c r="T16" s="105"/>
+      <c r="U16" s="105"/>
+      <c r="V16" s="105"/>
+      <c r="W16" s="105"/>
+      <c r="X16" s="105"/>
+      <c r="Y16" s="105"/>
+      <c r="Z16" s="105"/>
+      <c r="AA16" s="105"/>
+      <c r="AB16" s="105"/>
+      <c r="AC16" s="105"/>
+      <c r="AD16" s="105"/>
+      <c r="AE16" s="105"/>
+      <c r="AF16" s="107"/>
+      <c r="AG16" s="105"/>
+      <c r="AH16" s="105"/>
+      <c r="AI16" s="105"/>
+      <c r="AJ16" s="105"/>
+      <c r="AK16" s="105"/>
+      <c r="AL16" s="105"/>
+      <c r="AM16" s="105"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="148"/>
-      <c r="B17" s="132"/>
-      <c r="C17" s="132"/>
-      <c r="D17" s="131" t="s">
+      <c r="A17" s="155"/>
+      <c r="B17" s="157"/>
+      <c r="C17" s="157"/>
+      <c r="D17" s="105" t="s">
         <v>379</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="131" t="s">
+      <c r="E17" s="105"/>
+      <c r="F17" s="105" t="s">
         <v>406</v>
       </c>
-      <c r="G17" s="131" t="s">
-        <v>422</v>
-      </c>
-      <c r="H17" s="131"/>
-      <c r="I17" s="131"/>
-      <c r="J17" s="131"/>
-      <c r="K17" s="131"/>
-      <c r="L17" s="131"/>
-      <c r="M17" s="131"/>
-      <c r="N17" s="131"/>
-      <c r="O17" s="131"/>
-      <c r="P17" s="131"/>
-      <c r="Q17" s="131"/>
-      <c r="R17" s="131"/>
-      <c r="S17" s="131"/>
-      <c r="T17" s="131"/>
-      <c r="U17" s="131"/>
-      <c r="V17" s="131"/>
-      <c r="W17" s="131"/>
-      <c r="X17" s="131"/>
-      <c r="Y17" s="131"/>
-      <c r="Z17" s="131"/>
-      <c r="AA17" s="131"/>
-      <c r="AB17" s="131"/>
-      <c r="AC17" s="131"/>
-      <c r="AD17" s="131"/>
-      <c r="AE17" s="131"/>
-      <c r="AF17" s="137"/>
-      <c r="AG17" s="131"/>
-      <c r="AH17" s="131"/>
-      <c r="AI17" s="131"/>
-      <c r="AJ17" s="131"/>
-      <c r="AK17" s="131"/>
-      <c r="AL17" s="131"/>
-      <c r="AM17" s="131"/>
+      <c r="G17" s="105" t="s">
+        <v>451</v>
+      </c>
+      <c r="H17" s="105"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="105"/>
+      <c r="N17" s="105"/>
+      <c r="O17" s="105"/>
+      <c r="P17" s="105"/>
+      <c r="Q17" s="105"/>
+      <c r="R17" s="105"/>
+      <c r="S17" s="105"/>
+      <c r="T17" s="105"/>
+      <c r="U17" s="105"/>
+      <c r="V17" s="105"/>
+      <c r="W17" s="105"/>
+      <c r="X17" s="105"/>
+      <c r="Y17" s="105"/>
+      <c r="Z17" s="105"/>
+      <c r="AA17" s="105"/>
+      <c r="AB17" s="105"/>
+      <c r="AC17" s="105"/>
+      <c r="AD17" s="105"/>
+      <c r="AE17" s="105"/>
+      <c r="AF17" s="107"/>
+      <c r="AG17" s="105"/>
+      <c r="AH17" s="105"/>
+      <c r="AI17" s="105"/>
+      <c r="AJ17" s="105"/>
+      <c r="AK17" s="105"/>
+      <c r="AL17" s="105"/>
+      <c r="AM17" s="105"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="148"/>
-      <c r="B18" s="132"/>
-      <c r="C18" s="132"/>
-      <c r="D18" s="131" t="s">
+      <c r="A18" s="155"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="105" t="s">
         <v>380</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="131" t="s">
+      <c r="E18" s="105"/>
+      <c r="F18" s="105" t="s">
         <v>406</v>
       </c>
-      <c r="G18" s="131" t="s">
-        <v>422</v>
-      </c>
-      <c r="H18" s="131"/>
-      <c r="I18" s="131"/>
-      <c r="J18" s="131"/>
-      <c r="K18" s="131"/>
-      <c r="L18" s="131"/>
-      <c r="M18" s="131"/>
-      <c r="N18" s="131"/>
-      <c r="O18" s="131"/>
-      <c r="P18" s="131"/>
-      <c r="Q18" s="131"/>
-      <c r="R18" s="131"/>
-      <c r="S18" s="131"/>
-      <c r="T18" s="131"/>
-      <c r="U18" s="131"/>
-      <c r="V18" s="131"/>
-      <c r="W18" s="131"/>
-      <c r="X18" s="131"/>
-      <c r="Y18" s="131"/>
-      <c r="Z18" s="131"/>
-      <c r="AA18" s="131"/>
-      <c r="AB18" s="131"/>
-      <c r="AC18" s="131"/>
-      <c r="AD18" s="131"/>
-      <c r="AE18" s="131"/>
-      <c r="AF18" s="137"/>
-      <c r="AG18" s="131"/>
-      <c r="AH18" s="131"/>
-      <c r="AI18" s="131"/>
-      <c r="AJ18" s="131"/>
-      <c r="AK18" s="131"/>
-      <c r="AL18" s="131"/>
-      <c r="AM18" s="131"/>
+      <c r="G18" s="105" t="s">
+        <v>451</v>
+      </c>
+      <c r="H18" s="105"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="105"/>
+      <c r="N18" s="105"/>
+      <c r="O18" s="105"/>
+      <c r="P18" s="105"/>
+      <c r="Q18" s="105"/>
+      <c r="R18" s="105"/>
+      <c r="S18" s="105"/>
+      <c r="T18" s="105"/>
+      <c r="U18" s="105"/>
+      <c r="V18" s="105"/>
+      <c r="W18" s="105"/>
+      <c r="X18" s="105"/>
+      <c r="Y18" s="105"/>
+      <c r="Z18" s="105"/>
+      <c r="AA18" s="105"/>
+      <c r="AB18" s="105"/>
+      <c r="AC18" s="105"/>
+      <c r="AD18" s="105"/>
+      <c r="AE18" s="105"/>
+      <c r="AF18" s="107"/>
+      <c r="AG18" s="105"/>
+      <c r="AH18" s="105"/>
+      <c r="AI18" s="105"/>
+      <c r="AJ18" s="105"/>
+      <c r="AK18" s="105"/>
+      <c r="AL18" s="105"/>
+      <c r="AM18" s="105"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A19" s="148"/>
-      <c r="B19" s="132"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="131" t="s">
+      <c r="A19" s="155"/>
+      <c r="B19" s="157"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="105" t="s">
         <v>381</v>
       </c>
-      <c r="E19" s="131"/>
-      <c r="F19" s="131" t="s">
+      <c r="E19" s="105"/>
+      <c r="F19" s="105" t="s">
         <v>406</v>
       </c>
-      <c r="G19" s="131" t="s">
-        <v>422</v>
-      </c>
-      <c r="H19" s="131"/>
-      <c r="I19" s="131"/>
-      <c r="J19" s="131"/>
-      <c r="K19" s="131"/>
-      <c r="L19" s="131"/>
-      <c r="M19" s="131"/>
-      <c r="N19" s="131"/>
-      <c r="O19" s="131"/>
-      <c r="P19" s="131"/>
-      <c r="Q19" s="131"/>
-      <c r="R19" s="131"/>
-      <c r="S19" s="131"/>
-      <c r="T19" s="131"/>
-      <c r="U19" s="131"/>
-      <c r="V19" s="131"/>
-      <c r="W19" s="131"/>
-      <c r="X19" s="131"/>
-      <c r="Y19" s="131"/>
-      <c r="Z19" s="131"/>
-      <c r="AA19" s="131"/>
-      <c r="AB19" s="131"/>
-      <c r="AC19" s="131"/>
-      <c r="AD19" s="131"/>
-      <c r="AE19" s="131"/>
-      <c r="AF19" s="137"/>
-      <c r="AG19" s="131"/>
-      <c r="AH19" s="131"/>
-      <c r="AI19" s="131"/>
-      <c r="AJ19" s="131"/>
-      <c r="AK19" s="131"/>
-      <c r="AL19" s="131"/>
-      <c r="AM19" s="131"/>
+      <c r="G19" s="105" t="s">
+        <v>451</v>
+      </c>
+      <c r="H19" s="105"/>
+      <c r="I19" s="105"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="105"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="105"/>
+      <c r="N19" s="105"/>
+      <c r="O19" s="105"/>
+      <c r="P19" s="105"/>
+      <c r="Q19" s="105"/>
+      <c r="R19" s="105"/>
+      <c r="S19" s="105"/>
+      <c r="T19" s="105"/>
+      <c r="U19" s="105"/>
+      <c r="V19" s="105"/>
+      <c r="W19" s="105"/>
+      <c r="X19" s="105"/>
+      <c r="Y19" s="105"/>
+      <c r="Z19" s="105"/>
+      <c r="AA19" s="105"/>
+      <c r="AB19" s="105"/>
+      <c r="AC19" s="105"/>
+      <c r="AD19" s="105"/>
+      <c r="AE19" s="105"/>
+      <c r="AF19" s="107"/>
+      <c r="AG19" s="105"/>
+      <c r="AH19" s="105"/>
+      <c r="AI19" s="105"/>
+      <c r="AJ19" s="105"/>
+      <c r="AK19" s="105"/>
+      <c r="AL19" s="105"/>
+      <c r="AM19" s="105"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" s="148"/>
-      <c r="B20" s="132"/>
-      <c r="C20" s="132"/>
-      <c r="D20" s="131" t="s">
+      <c r="A20" s="155"/>
+      <c r="B20" s="157"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="105" t="s">
         <v>407</v>
       </c>
-      <c r="E20" s="131"/>
-      <c r="F20" s="131" t="s">
+      <c r="E20" s="105"/>
+      <c r="F20" s="105" t="s">
         <v>408</v>
       </c>
-      <c r="G20" s="131" t="s">
+      <c r="G20" s="105" t="s">
+        <v>464</v>
+      </c>
+      <c r="H20" s="105"/>
+      <c r="I20" s="105"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="105"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="105"/>
+      <c r="N20" s="105"/>
+      <c r="O20" s="105"/>
+      <c r="P20" s="105"/>
+      <c r="Q20" s="105"/>
+      <c r="R20" s="105"/>
+      <c r="S20" s="105"/>
+      <c r="T20" s="105"/>
+      <c r="U20" s="105"/>
+      <c r="V20" s="105"/>
+      <c r="W20" s="105"/>
+      <c r="X20" s="105"/>
+      <c r="Y20" s="105"/>
+      <c r="Z20" s="105"/>
+      <c r="AA20" s="105"/>
+      <c r="AB20" s="105"/>
+      <c r="AC20" s="105"/>
+      <c r="AD20" s="105"/>
+      <c r="AE20" s="105"/>
+      <c r="AF20" s="105"/>
+      <c r="AG20" s="107"/>
+      <c r="AH20" s="105"/>
+      <c r="AI20" s="105"/>
+      <c r="AJ20" s="105"/>
+      <c r="AK20" s="105"/>
+      <c r="AL20" s="105"/>
+      <c r="AM20" s="105"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A21" s="155"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157" t="s">
+        <v>382</v>
+      </c>
+      <c r="D21" s="105" t="s">
+        <v>383</v>
+      </c>
+      <c r="E21" s="105"/>
+      <c r="F21" s="105" t="s">
         <v>452</v>
       </c>
-      <c r="H20" s="131"/>
-      <c r="I20" s="131"/>
-      <c r="J20" s="131"/>
-      <c r="K20" s="131"/>
-      <c r="L20" s="131"/>
-      <c r="M20" s="131"/>
-      <c r="N20" s="131"/>
-      <c r="O20" s="131"/>
-      <c r="P20" s="131"/>
-      <c r="Q20" s="131"/>
-      <c r="R20" s="131"/>
-      <c r="S20" s="131"/>
-      <c r="T20" s="131"/>
-      <c r="U20" s="131"/>
-      <c r="V20" s="131"/>
-      <c r="W20" s="131"/>
-      <c r="X20" s="131"/>
-      <c r="Y20" s="131"/>
-      <c r="Z20" s="131"/>
-      <c r="AA20" s="131"/>
-      <c r="AB20" s="131"/>
-      <c r="AC20" s="131"/>
-      <c r="AD20" s="131"/>
-      <c r="AE20" s="131"/>
-      <c r="AF20" s="131"/>
-      <c r="AG20" s="137"/>
-      <c r="AH20" s="131"/>
-      <c r="AI20" s="131"/>
-      <c r="AJ20" s="131"/>
-      <c r="AK20" s="131"/>
-      <c r="AL20" s="131"/>
-      <c r="AM20" s="131"/>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="148"/>
-      <c r="B21" s="132"/>
-      <c r="C21" s="132" t="s">
-        <v>382</v>
-      </c>
-      <c r="D21" s="131" t="s">
-        <v>383</v>
-      </c>
-      <c r="E21" s="131"/>
-      <c r="F21" s="131" t="s">
+      <c r="G21" s="105" t="s">
         <v>453</v>
       </c>
-      <c r="G21" s="131" t="s">
+      <c r="H21" s="105"/>
+      <c r="I21" s="105"/>
+      <c r="J21" s="105"/>
+      <c r="K21" s="105"/>
+      <c r="L21" s="105"/>
+      <c r="M21" s="105"/>
+      <c r="N21" s="105"/>
+      <c r="O21" s="105"/>
+      <c r="P21" s="105"/>
+      <c r="Q21" s="105"/>
+      <c r="R21" s="105"/>
+      <c r="S21" s="105"/>
+      <c r="T21" s="105"/>
+      <c r="U21" s="105"/>
+      <c r="V21" s="105"/>
+      <c r="W21" s="105"/>
+      <c r="X21" s="105"/>
+      <c r="Y21" s="105"/>
+      <c r="Z21" s="105"/>
+      <c r="AA21" s="105"/>
+      <c r="AB21" s="105"/>
+      <c r="AC21" s="105"/>
+      <c r="AD21" s="105"/>
+      <c r="AE21" s="105"/>
+      <c r="AF21" s="105"/>
+      <c r="AG21" s="105"/>
+      <c r="AH21" s="105"/>
+      <c r="AI21" s="105"/>
+      <c r="AJ21" s="105"/>
+      <c r="AK21" s="105"/>
+      <c r="AL21" s="105"/>
+      <c r="AM21" s="105"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A22" s="155"/>
+      <c r="B22" s="157"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="105" t="s">
+        <v>384</v>
+      </c>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105" t="s">
+        <v>452</v>
+      </c>
+      <c r="G22" s="105" t="s">
+        <v>453</v>
+      </c>
+      <c r="H22" s="105"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="105"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="105"/>
+      <c r="O22" s="105"/>
+      <c r="P22" s="105"/>
+      <c r="Q22" s="105"/>
+      <c r="R22" s="105"/>
+      <c r="S22" s="105"/>
+      <c r="T22" s="105"/>
+      <c r="U22" s="105"/>
+      <c r="V22" s="105"/>
+      <c r="W22" s="105"/>
+      <c r="X22" s="105"/>
+      <c r="Y22" s="105"/>
+      <c r="Z22" s="105"/>
+      <c r="AA22" s="105"/>
+      <c r="AB22" s="105"/>
+      <c r="AC22" s="105"/>
+      <c r="AD22" s="105"/>
+      <c r="AE22" s="105"/>
+      <c r="AF22" s="105"/>
+      <c r="AG22" s="105"/>
+      <c r="AH22" s="105"/>
+      <c r="AI22" s="105"/>
+      <c r="AJ22" s="105"/>
+      <c r="AK22" s="105"/>
+      <c r="AL22" s="105"/>
+      <c r="AM22" s="105"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A23" s="155"/>
+      <c r="B23" s="157"/>
+      <c r="C23" s="157"/>
+      <c r="D23" s="105" t="s">
+        <v>385</v>
+      </c>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105" t="s">
+        <v>452</v>
+      </c>
+      <c r="G23" s="105" t="s">
+        <v>453</v>
+      </c>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="105"/>
+      <c r="N23" s="105"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="105"/>
+      <c r="Q23" s="105"/>
+      <c r="R23" s="105"/>
+      <c r="S23" s="105"/>
+      <c r="T23" s="105"/>
+      <c r="U23" s="105"/>
+      <c r="V23" s="105"/>
+      <c r="W23" s="105"/>
+      <c r="X23" s="105"/>
+      <c r="Y23" s="105"/>
+      <c r="Z23" s="105"/>
+      <c r="AA23" s="105"/>
+      <c r="AB23" s="105"/>
+      <c r="AC23" s="105"/>
+      <c r="AD23" s="105"/>
+      <c r="AE23" s="105"/>
+      <c r="AF23" s="105"/>
+      <c r="AG23" s="105"/>
+      <c r="AH23" s="105"/>
+      <c r="AI23" s="105"/>
+      <c r="AJ23" s="105"/>
+      <c r="AK23" s="105"/>
+      <c r="AL23" s="105"/>
+      <c r="AM23" s="105"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A24" s="155"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="105" t="s">
+        <v>369</v>
+      </c>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105" t="s">
         <v>454</v>
       </c>
-      <c r="H21" s="131"/>
-      <c r="I21" s="131"/>
-      <c r="J21" s="131"/>
-      <c r="K21" s="131"/>
-      <c r="L21" s="131"/>
-      <c r="M21" s="131"/>
-      <c r="N21" s="131"/>
-      <c r="O21" s="131"/>
-      <c r="P21" s="131"/>
-      <c r="Q21" s="131"/>
-      <c r="R21" s="131"/>
-      <c r="S21" s="131"/>
-      <c r="T21" s="131"/>
-      <c r="U21" s="131"/>
-      <c r="V21" s="131"/>
-      <c r="W21" s="131"/>
-      <c r="X21" s="131"/>
-      <c r="Y21" s="131"/>
-      <c r="Z21" s="131"/>
-      <c r="AA21" s="131"/>
-      <c r="AB21" s="131"/>
-      <c r="AC21" s="131"/>
-      <c r="AD21" s="131"/>
-      <c r="AE21" s="131"/>
-      <c r="AF21" s="131"/>
-      <c r="AG21" s="131"/>
-      <c r="AH21" s="131"/>
-      <c r="AI21" s="131"/>
-      <c r="AJ21" s="131"/>
-      <c r="AK21" s="131"/>
-      <c r="AL21" s="131"/>
-      <c r="AM21" s="131"/>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="148"/>
-      <c r="B22" s="132"/>
-      <c r="C22" s="132"/>
-      <c r="D22" s="131" t="s">
-        <v>384</v>
-      </c>
-      <c r="E22" s="131"/>
-      <c r="F22" s="131" t="s">
-        <v>453</v>
-      </c>
-      <c r="G22" s="131" t="s">
-        <v>454</v>
-      </c>
-      <c r="H22" s="131"/>
-      <c r="I22" s="131"/>
-      <c r="J22" s="131"/>
-      <c r="K22" s="131"/>
-      <c r="L22" s="131"/>
-      <c r="M22" s="131"/>
-      <c r="N22" s="131"/>
-      <c r="O22" s="131"/>
-      <c r="P22" s="131"/>
-      <c r="Q22" s="131"/>
-      <c r="R22" s="131"/>
-      <c r="S22" s="131"/>
-      <c r="T22" s="131"/>
-      <c r="U22" s="131"/>
-      <c r="V22" s="131"/>
-      <c r="W22" s="131"/>
-      <c r="X22" s="131"/>
-      <c r="Y22" s="131"/>
-      <c r="Z22" s="131"/>
-      <c r="AA22" s="131"/>
-      <c r="AB22" s="131"/>
-      <c r="AC22" s="131"/>
-      <c r="AD22" s="131"/>
-      <c r="AE22" s="131"/>
-      <c r="AF22" s="131"/>
-      <c r="AG22" s="131"/>
-      <c r="AH22" s="131"/>
-      <c r="AI22" s="131"/>
-      <c r="AJ22" s="131"/>
-      <c r="AK22" s="131"/>
-      <c r="AL22" s="131"/>
-      <c r="AM22" s="131"/>
-    </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A23" s="148"/>
-      <c r="B23" s="132"/>
-      <c r="C23" s="132"/>
-      <c r="D23" s="131" t="s">
-        <v>385</v>
-      </c>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131" t="s">
-        <v>453</v>
-      </c>
-      <c r="G23" s="131" t="s">
-        <v>454</v>
-      </c>
-      <c r="H23" s="131"/>
-      <c r="I23" s="131"/>
-      <c r="J23" s="131"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="131"/>
-      <c r="M23" s="131"/>
-      <c r="N23" s="131"/>
-      <c r="O23" s="131"/>
-      <c r="P23" s="131"/>
-      <c r="Q23" s="131"/>
-      <c r="R23" s="131"/>
-      <c r="S23" s="131"/>
-      <c r="T23" s="131"/>
-      <c r="U23" s="131"/>
-      <c r="V23" s="131"/>
-      <c r="W23" s="131"/>
-      <c r="X23" s="131"/>
-      <c r="Y23" s="131"/>
-      <c r="Z23" s="131"/>
-      <c r="AA23" s="131"/>
-      <c r="AB23" s="131"/>
-      <c r="AC23" s="131"/>
-      <c r="AD23" s="131"/>
-      <c r="AE23" s="131"/>
-      <c r="AF23" s="131"/>
-      <c r="AG23" s="131"/>
-      <c r="AH23" s="131"/>
-      <c r="AI23" s="131"/>
-      <c r="AJ23" s="131"/>
-      <c r="AK23" s="131"/>
-      <c r="AL23" s="131"/>
-      <c r="AM23" s="131"/>
-    </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="148"/>
-      <c r="B24" s="132"/>
-      <c r="C24" s="131" t="s">
-        <v>369</v>
-      </c>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131" t="s">
+      <c r="G24" s="105" t="s">
         <v>455</v>
       </c>
-      <c r="G24" s="131" t="s">
-        <v>456</v>
-      </c>
-      <c r="H24" s="131"/>
-      <c r="I24" s="131"/>
-      <c r="J24" s="131"/>
-      <c r="K24" s="131"/>
-      <c r="L24" s="131"/>
-      <c r="M24" s="131"/>
-      <c r="N24" s="131"/>
-      <c r="O24" s="131"/>
-      <c r="P24" s="131"/>
-      <c r="Q24" s="131"/>
-      <c r="R24" s="131"/>
-      <c r="S24" s="131"/>
-      <c r="T24" s="131"/>
-      <c r="U24" s="131"/>
-      <c r="V24" s="131"/>
-      <c r="W24" s="131"/>
-      <c r="X24" s="131"/>
-      <c r="Y24" s="131"/>
-      <c r="Z24" s="131"/>
-      <c r="AA24" s="131"/>
-      <c r="AB24" s="131"/>
-      <c r="AC24" s="131"/>
-      <c r="AD24" s="131"/>
-      <c r="AE24" s="131"/>
-      <c r="AF24" s="131"/>
-      <c r="AG24" s="131"/>
-      <c r="AH24" s="131"/>
-      <c r="AI24" s="131"/>
-      <c r="AJ24" s="131"/>
-      <c r="AK24" s="131"/>
-      <c r="AL24" s="131"/>
-      <c r="AM24" s="131"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="105"/>
+      <c r="N24" s="105"/>
+      <c r="O24" s="105"/>
+      <c r="P24" s="105"/>
+      <c r="Q24" s="105"/>
+      <c r="R24" s="105"/>
+      <c r="S24" s="105"/>
+      <c r="T24" s="105"/>
+      <c r="U24" s="105"/>
+      <c r="V24" s="105"/>
+      <c r="W24" s="105"/>
+      <c r="X24" s="105"/>
+      <c r="Y24" s="105"/>
+      <c r="Z24" s="105"/>
+      <c r="AA24" s="105"/>
+      <c r="AB24" s="105"/>
+      <c r="AC24" s="105"/>
+      <c r="AD24" s="105"/>
+      <c r="AE24" s="105"/>
+      <c r="AF24" s="105"/>
+      <c r="AG24" s="105"/>
+      <c r="AH24" s="105"/>
+      <c r="AI24" s="105"/>
+      <c r="AJ24" s="105"/>
+      <c r="AK24" s="105"/>
+      <c r="AL24" s="105"/>
+      <c r="AM24" s="105"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A25" s="148"/>
-      <c r="B25" s="132"/>
-      <c r="C25" s="132" t="s">
+      <c r="A25" s="155"/>
+      <c r="B25" s="157"/>
+      <c r="C25" s="157" t="s">
         <v>391</v>
       </c>
-      <c r="D25" s="132" t="s">
+      <c r="D25" s="157" t="s">
         <v>392</v>
       </c>
-      <c r="E25" s="131" t="s">
+      <c r="E25" s="105" t="s">
         <v>393</v>
       </c>
-      <c r="F25" s="131" t="s">
+      <c r="F25" s="105" t="s">
+        <v>449</v>
+      </c>
+      <c r="G25" s="105" t="s">
+        <v>458</v>
+      </c>
+      <c r="H25" s="105"/>
+      <c r="I25" s="105"/>
+      <c r="J25" s="105"/>
+      <c r="K25" s="105"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="105"/>
+      <c r="N25" s="105"/>
+      <c r="O25" s="105"/>
+      <c r="P25" s="105"/>
+      <c r="Q25" s="105"/>
+      <c r="R25" s="105"/>
+      <c r="S25" s="105"/>
+      <c r="T25" s="105"/>
+      <c r="U25" s="105"/>
+      <c r="V25" s="105"/>
+      <c r="W25" s="105"/>
+      <c r="X25" s="105"/>
+      <c r="Y25" s="105"/>
+      <c r="Z25" s="105"/>
+      <c r="AA25" s="105"/>
+      <c r="AB25" s="105"/>
+      <c r="AC25" s="105"/>
+      <c r="AD25" s="105"/>
+      <c r="AE25" s="105"/>
+      <c r="AF25" s="105"/>
+      <c r="AG25" s="105"/>
+      <c r="AH25" s="105"/>
+      <c r="AI25" s="105"/>
+      <c r="AJ25" s="105"/>
+      <c r="AK25" s="105"/>
+      <c r="AL25" s="105"/>
+      <c r="AM25" s="105"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A26" s="155"/>
+      <c r="B26" s="157"/>
+      <c r="C26" s="157"/>
+      <c r="D26" s="157"/>
+      <c r="E26" s="105" t="s">
+        <v>394</v>
+      </c>
+      <c r="F26" s="105" t="s">
+        <v>449</v>
+      </c>
+      <c r="G26" s="105" t="s">
+        <v>458</v>
+      </c>
+      <c r="H26" s="105"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="105"/>
+      <c r="K26" s="105"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="105"/>
+      <c r="N26" s="105"/>
+      <c r="O26" s="105"/>
+      <c r="P26" s="105"/>
+      <c r="Q26" s="105"/>
+      <c r="R26" s="105"/>
+      <c r="S26" s="105"/>
+      <c r="T26" s="105"/>
+      <c r="U26" s="105"/>
+      <c r="V26" s="105"/>
+      <c r="W26" s="105"/>
+      <c r="X26" s="105"/>
+      <c r="Y26" s="105"/>
+      <c r="Z26" s="105"/>
+      <c r="AA26" s="105"/>
+      <c r="AB26" s="105"/>
+      <c r="AC26" s="105"/>
+      <c r="AD26" s="105"/>
+      <c r="AE26" s="105"/>
+      <c r="AF26" s="105"/>
+      <c r="AG26" s="105"/>
+      <c r="AH26" s="105"/>
+      <c r="AI26" s="105"/>
+      <c r="AJ26" s="105"/>
+      <c r="AK26" s="105"/>
+      <c r="AL26" s="105"/>
+      <c r="AM26" s="105"/>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A27" s="155"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157" t="s">
+        <v>395</v>
+      </c>
+      <c r="E27" s="105" t="s">
+        <v>388</v>
+      </c>
+      <c r="F27" s="105" t="s">
+        <v>459</v>
+      </c>
+      <c r="G27" s="105" t="s">
+        <v>460</v>
+      </c>
+      <c r="H27" s="105"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="105"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="105"/>
+      <c r="N27" s="105"/>
+      <c r="O27" s="105"/>
+      <c r="P27" s="105"/>
+      <c r="Q27" s="105"/>
+      <c r="R27" s="105"/>
+      <c r="S27" s="105"/>
+      <c r="T27" s="105"/>
+      <c r="U27" s="105"/>
+      <c r="V27" s="105"/>
+      <c r="W27" s="105"/>
+      <c r="X27" s="105"/>
+      <c r="Y27" s="105"/>
+      <c r="Z27" s="105"/>
+      <c r="AA27" s="105"/>
+      <c r="AB27" s="105"/>
+      <c r="AC27" s="105"/>
+      <c r="AD27" s="105"/>
+      <c r="AE27" s="105"/>
+      <c r="AF27" s="105"/>
+      <c r="AG27" s="105"/>
+      <c r="AH27" s="105"/>
+      <c r="AI27" s="105"/>
+      <c r="AJ27" s="105"/>
+      <c r="AK27" s="105"/>
+      <c r="AL27" s="105"/>
+      <c r="AM27" s="105"/>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A28" s="155"/>
+      <c r="B28" s="157"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="105" t="s">
+        <v>389</v>
+      </c>
+      <c r="F28" s="105" t="s">
+        <v>459</v>
+      </c>
+      <c r="G28" s="105" t="s">
+        <v>460</v>
+      </c>
+      <c r="H28" s="105"/>
+      <c r="I28" s="105"/>
+      <c r="J28" s="105"/>
+      <c r="K28" s="105"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="105"/>
+      <c r="N28" s="105"/>
+      <c r="O28" s="105"/>
+      <c r="P28" s="105"/>
+      <c r="Q28" s="105"/>
+      <c r="R28" s="105"/>
+      <c r="S28" s="105"/>
+      <c r="T28" s="105"/>
+      <c r="U28" s="105"/>
+      <c r="V28" s="105"/>
+      <c r="W28" s="105"/>
+      <c r="X28" s="105"/>
+      <c r="Y28" s="105"/>
+      <c r="Z28" s="105"/>
+      <c r="AA28" s="105"/>
+      <c r="AB28" s="105"/>
+      <c r="AC28" s="105"/>
+      <c r="AD28" s="105"/>
+      <c r="AE28" s="105"/>
+      <c r="AF28" s="105"/>
+      <c r="AG28" s="105"/>
+      <c r="AH28" s="105"/>
+      <c r="AI28" s="105"/>
+      <c r="AJ28" s="105"/>
+      <c r="AK28" s="105"/>
+      <c r="AL28" s="105"/>
+      <c r="AM28" s="105"/>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A29" s="155"/>
+      <c r="B29" s="157"/>
+      <c r="C29" s="157"/>
+      <c r="D29" s="157"/>
+      <c r="E29" s="105" t="s">
+        <v>387</v>
+      </c>
+      <c r="F29" s="105" t="s">
+        <v>459</v>
+      </c>
+      <c r="G29" s="105" t="s">
+        <v>460</v>
+      </c>
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="105"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="105"/>
+      <c r="N29" s="105"/>
+      <c r="O29" s="105"/>
+      <c r="P29" s="105"/>
+      <c r="Q29" s="105"/>
+      <c r="R29" s="105"/>
+      <c r="S29" s="105"/>
+      <c r="T29" s="105"/>
+      <c r="U29" s="105"/>
+      <c r="V29" s="105"/>
+      <c r="W29" s="105"/>
+      <c r="X29" s="105"/>
+      <c r="Y29" s="105"/>
+      <c r="Z29" s="105"/>
+      <c r="AA29" s="105"/>
+      <c r="AB29" s="105"/>
+      <c r="AC29" s="105"/>
+      <c r="AD29" s="105"/>
+      <c r="AE29" s="105"/>
+      <c r="AF29" s="105"/>
+      <c r="AG29" s="105"/>
+      <c r="AH29" s="105"/>
+      <c r="AI29" s="105"/>
+      <c r="AJ29" s="105"/>
+      <c r="AK29" s="105"/>
+      <c r="AL29" s="105"/>
+      <c r="AM29" s="105"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A30" s="155"/>
+      <c r="B30" s="157"/>
+      <c r="C30" s="157"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="105" t="s">
+        <v>390</v>
+      </c>
+      <c r="F30" s="105" t="s">
+        <v>459</v>
+      </c>
+      <c r="G30" s="105" t="s">
+        <v>460</v>
+      </c>
+      <c r="H30" s="105"/>
+      <c r="I30" s="105"/>
+      <c r="J30" s="105"/>
+      <c r="K30" s="105"/>
+      <c r="L30" s="105"/>
+      <c r="M30" s="105"/>
+      <c r="N30" s="105"/>
+      <c r="O30" s="105"/>
+      <c r="P30" s="105"/>
+      <c r="Q30" s="105"/>
+      <c r="R30" s="105"/>
+      <c r="S30" s="105"/>
+      <c r="T30" s="105"/>
+      <c r="U30" s="105"/>
+      <c r="V30" s="105"/>
+      <c r="W30" s="105"/>
+      <c r="X30" s="105"/>
+      <c r="Y30" s="105"/>
+      <c r="Z30" s="105"/>
+      <c r="AA30" s="105"/>
+      <c r="AB30" s="105"/>
+      <c r="AC30" s="105"/>
+      <c r="AD30" s="105"/>
+      <c r="AE30" s="105"/>
+      <c r="AF30" s="105"/>
+      <c r="AG30" s="105"/>
+      <c r="AH30" s="105"/>
+      <c r="AI30" s="105"/>
+      <c r="AJ30" s="105"/>
+      <c r="AK30" s="105"/>
+      <c r="AL30" s="105"/>
+      <c r="AM30" s="105"/>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A31" s="156"/>
+      <c r="B31" s="105" t="s">
+        <v>403</v>
+      </c>
+      <c r="C31" s="157" t="s">
+        <v>335</v>
+      </c>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="105" t="s">
+        <v>461</v>
+      </c>
+      <c r="G31" s="105" t="s">
         <v>450</v>
       </c>
-      <c r="G25" s="131" t="s">
-        <v>459</v>
-      </c>
-      <c r="H25" s="131"/>
-      <c r="I25" s="131"/>
-      <c r="J25" s="131"/>
-      <c r="K25" s="131"/>
-      <c r="L25" s="131"/>
-      <c r="M25" s="131"/>
-      <c r="N25" s="131"/>
-      <c r="O25" s="131"/>
-      <c r="P25" s="131"/>
-      <c r="Q25" s="131"/>
-      <c r="R25" s="131"/>
-      <c r="S25" s="131"/>
-      <c r="T25" s="131"/>
-      <c r="U25" s="131"/>
-      <c r="V25" s="131"/>
-      <c r="W25" s="131"/>
-      <c r="X25" s="131"/>
-      <c r="Y25" s="131"/>
-      <c r="Z25" s="131"/>
-      <c r="AA25" s="131"/>
-      <c r="AB25" s="131"/>
-      <c r="AC25" s="131"/>
-      <c r="AD25" s="131"/>
-      <c r="AE25" s="131"/>
-      <c r="AF25" s="131"/>
-      <c r="AG25" s="131"/>
-      <c r="AH25" s="131"/>
-      <c r="AI25" s="131"/>
-      <c r="AJ25" s="131"/>
-      <c r="AK25" s="131"/>
-      <c r="AL25" s="131"/>
-      <c r="AM25" s="131"/>
-    </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="148"/>
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="131" t="s">
-        <v>394</v>
-      </c>
-      <c r="F26" s="131" t="s">
-        <v>450</v>
-      </c>
-      <c r="G26" s="131" t="s">
-        <v>459</v>
-      </c>
-      <c r="H26" s="131"/>
-      <c r="I26" s="131"/>
-      <c r="J26" s="131"/>
-      <c r="K26" s="131"/>
-      <c r="L26" s="131"/>
-      <c r="M26" s="131"/>
-      <c r="N26" s="131"/>
-      <c r="O26" s="131"/>
-      <c r="P26" s="131"/>
-      <c r="Q26" s="131"/>
-      <c r="R26" s="131"/>
-      <c r="S26" s="131"/>
-      <c r="T26" s="131"/>
-      <c r="U26" s="131"/>
-      <c r="V26" s="131"/>
-      <c r="W26" s="131"/>
-      <c r="X26" s="131"/>
-      <c r="Y26" s="131"/>
-      <c r="Z26" s="131"/>
-      <c r="AA26" s="131"/>
-      <c r="AB26" s="131"/>
-      <c r="AC26" s="131"/>
-      <c r="AD26" s="131"/>
-      <c r="AE26" s="131"/>
-      <c r="AF26" s="131"/>
-      <c r="AG26" s="131"/>
-      <c r="AH26" s="131"/>
-      <c r="AI26" s="131"/>
-      <c r="AJ26" s="131"/>
-      <c r="AK26" s="131"/>
-      <c r="AL26" s="131"/>
-      <c r="AM26" s="131"/>
-    </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A27" s="148"/>
-      <c r="B27" s="132"/>
-      <c r="C27" s="132"/>
-      <c r="D27" s="132" t="s">
-        <v>395</v>
-      </c>
-      <c r="E27" s="131" t="s">
-        <v>388</v>
-      </c>
-      <c r="F27" s="131" t="s">
-        <v>460</v>
-      </c>
-      <c r="G27" s="131" t="s">
-        <v>461</v>
-      </c>
-      <c r="H27" s="131"/>
-      <c r="I27" s="131"/>
-      <c r="J27" s="131"/>
-      <c r="K27" s="131"/>
-      <c r="L27" s="131"/>
-      <c r="M27" s="131"/>
-      <c r="N27" s="131"/>
-      <c r="O27" s="131"/>
-      <c r="P27" s="131"/>
-      <c r="Q27" s="131"/>
-      <c r="R27" s="131"/>
-      <c r="S27" s="131"/>
-      <c r="T27" s="131"/>
-      <c r="U27" s="131"/>
-      <c r="V27" s="131"/>
-      <c r="W27" s="131"/>
-      <c r="X27" s="131"/>
-      <c r="Y27" s="131"/>
-      <c r="Z27" s="131"/>
-      <c r="AA27" s="131"/>
-      <c r="AB27" s="131"/>
-      <c r="AC27" s="131"/>
-      <c r="AD27" s="131"/>
-      <c r="AE27" s="131"/>
-      <c r="AF27" s="131"/>
-      <c r="AG27" s="131"/>
-      <c r="AH27" s="131"/>
-      <c r="AI27" s="131"/>
-      <c r="AJ27" s="131"/>
-      <c r="AK27" s="131"/>
-      <c r="AL27" s="131"/>
-      <c r="AM27" s="131"/>
-    </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="148"/>
-      <c r="B28" s="132"/>
-      <c r="C28" s="132"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="131" t="s">
-        <v>389</v>
-      </c>
-      <c r="F28" s="131" t="s">
-        <v>460</v>
-      </c>
-      <c r="G28" s="131" t="s">
-        <v>461</v>
-      </c>
-      <c r="H28" s="131"/>
-      <c r="I28" s="131"/>
-      <c r="J28" s="131"/>
-      <c r="K28" s="131"/>
-      <c r="L28" s="131"/>
-      <c r="M28" s="131"/>
-      <c r="N28" s="131"/>
-      <c r="O28" s="131"/>
-      <c r="P28" s="131"/>
-      <c r="Q28" s="131"/>
-      <c r="R28" s="131"/>
-      <c r="S28" s="131"/>
-      <c r="T28" s="131"/>
-      <c r="U28" s="131"/>
-      <c r="V28" s="131"/>
-      <c r="W28" s="131"/>
-      <c r="X28" s="131"/>
-      <c r="Y28" s="131"/>
-      <c r="Z28" s="131"/>
-      <c r="AA28" s="131"/>
-      <c r="AB28" s="131"/>
-      <c r="AC28" s="131"/>
-      <c r="AD28" s="131"/>
-      <c r="AE28" s="131"/>
-      <c r="AF28" s="131"/>
-      <c r="AG28" s="131"/>
-      <c r="AH28" s="131"/>
-      <c r="AI28" s="131"/>
-      <c r="AJ28" s="131"/>
-      <c r="AK28" s="131"/>
-      <c r="AL28" s="131"/>
-      <c r="AM28" s="131"/>
-    </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="148"/>
-      <c r="B29" s="132"/>
-      <c r="C29" s="132"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="131" t="s">
-        <v>387</v>
-      </c>
-      <c r="F29" s="131" t="s">
-        <v>460</v>
-      </c>
-      <c r="G29" s="131" t="s">
-        <v>461</v>
-      </c>
-      <c r="H29" s="131"/>
-      <c r="I29" s="131"/>
-      <c r="J29" s="131"/>
-      <c r="K29" s="131"/>
-      <c r="L29" s="131"/>
-      <c r="M29" s="131"/>
-      <c r="N29" s="131"/>
-      <c r="O29" s="131"/>
-      <c r="P29" s="131"/>
-      <c r="Q29" s="131"/>
-      <c r="R29" s="131"/>
-      <c r="S29" s="131"/>
-      <c r="T29" s="131"/>
-      <c r="U29" s="131"/>
-      <c r="V29" s="131"/>
-      <c r="W29" s="131"/>
-      <c r="X29" s="131"/>
-      <c r="Y29" s="131"/>
-      <c r="Z29" s="131"/>
-      <c r="AA29" s="131"/>
-      <c r="AB29" s="131"/>
-      <c r="AC29" s="131"/>
-      <c r="AD29" s="131"/>
-      <c r="AE29" s="131"/>
-      <c r="AF29" s="131"/>
-      <c r="AG29" s="131"/>
-      <c r="AH29" s="131"/>
-      <c r="AI29" s="131"/>
-      <c r="AJ29" s="131"/>
-      <c r="AK29" s="131"/>
-      <c r="AL29" s="131"/>
-      <c r="AM29" s="131"/>
-    </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="148"/>
-      <c r="B30" s="132"/>
-      <c r="C30" s="132"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="131" t="s">
-        <v>390</v>
-      </c>
-      <c r="F30" s="131" t="s">
-        <v>460</v>
-      </c>
-      <c r="G30" s="131" t="s">
-        <v>461</v>
-      </c>
-      <c r="H30" s="131"/>
-      <c r="I30" s="131"/>
-      <c r="J30" s="131"/>
-      <c r="K30" s="131"/>
-      <c r="L30" s="131"/>
-      <c r="M30" s="131"/>
-      <c r="N30" s="131"/>
-      <c r="O30" s="131"/>
-      <c r="P30" s="131"/>
-      <c r="Q30" s="131"/>
-      <c r="R30" s="131"/>
-      <c r="S30" s="131"/>
-      <c r="T30" s="131"/>
-      <c r="U30" s="131"/>
-      <c r="V30" s="131"/>
-      <c r="W30" s="131"/>
-      <c r="X30" s="131"/>
-      <c r="Y30" s="131"/>
-      <c r="Z30" s="131"/>
-      <c r="AA30" s="131"/>
-      <c r="AB30" s="131"/>
-      <c r="AC30" s="131"/>
-      <c r="AD30" s="131"/>
-      <c r="AE30" s="131"/>
-      <c r="AF30" s="131"/>
-      <c r="AG30" s="131"/>
-      <c r="AH30" s="131"/>
-      <c r="AI30" s="131"/>
-      <c r="AJ30" s="131"/>
-      <c r="AK30" s="131"/>
-      <c r="AL30" s="131"/>
-      <c r="AM30" s="131"/>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A31" s="149"/>
-      <c r="B31" s="131" t="s">
-        <v>403</v>
-      </c>
-      <c r="C31" s="132" t="s">
-        <v>335</v>
-      </c>
-      <c r="D31" s="132"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="131" t="s">
+      <c r="H31" s="105"/>
+      <c r="I31" s="105"/>
+      <c r="J31" s="105"/>
+      <c r="K31" s="105"/>
+      <c r="L31" s="105"/>
+      <c r="M31" s="105"/>
+      <c r="N31" s="105"/>
+      <c r="O31" s="105"/>
+      <c r="P31" s="105"/>
+      <c r="Q31" s="105"/>
+      <c r="R31" s="105"/>
+      <c r="S31" s="105"/>
+      <c r="T31" s="105"/>
+      <c r="U31" s="105"/>
+      <c r="V31" s="105"/>
+      <c r="W31" s="105"/>
+      <c r="X31" s="105"/>
+      <c r="Y31" s="105"/>
+      <c r="Z31" s="105"/>
+      <c r="AA31" s="105"/>
+      <c r="AB31" s="105"/>
+      <c r="AC31" s="105"/>
+      <c r="AD31" s="105"/>
+      <c r="AE31" s="105"/>
+      <c r="AF31" s="105"/>
+      <c r="AG31" s="105"/>
+      <c r="AH31" s="105"/>
+      <c r="AI31" s="105"/>
+      <c r="AJ31" s="105"/>
+      <c r="AK31" s="105"/>
+      <c r="AL31" s="105"/>
+      <c r="AM31" s="105"/>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A32" s="105" t="s">
+        <v>356</v>
+      </c>
+      <c r="B32" s="106"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="105" t="s">
         <v>462</v>
       </c>
-      <c r="G31" s="131" t="s">
-        <v>451</v>
-      </c>
-      <c r="H31" s="131"/>
-      <c r="I31" s="131"/>
-      <c r="J31" s="131"/>
-      <c r="K31" s="131"/>
-      <c r="L31" s="131"/>
-      <c r="M31" s="131"/>
-      <c r="N31" s="131"/>
-      <c r="O31" s="131"/>
-      <c r="P31" s="131"/>
-      <c r="Q31" s="131"/>
-      <c r="R31" s="131"/>
-      <c r="S31" s="131"/>
-      <c r="T31" s="131"/>
-      <c r="U31" s="131"/>
-      <c r="V31" s="131"/>
-      <c r="W31" s="131"/>
-      <c r="X31" s="131"/>
-      <c r="Y31" s="131"/>
-      <c r="Z31" s="131"/>
-      <c r="AA31" s="131"/>
-      <c r="AB31" s="131"/>
-      <c r="AC31" s="131"/>
-      <c r="AD31" s="131"/>
-      <c r="AE31" s="131"/>
-      <c r="AF31" s="131"/>
-      <c r="AG31" s="131"/>
-      <c r="AH31" s="131"/>
-      <c r="AI31" s="131"/>
-      <c r="AJ31" s="131"/>
-      <c r="AK31" s="131"/>
-      <c r="AL31" s="131"/>
-      <c r="AM31" s="131"/>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A32" s="131" t="s">
-        <v>356</v>
-      </c>
-      <c r="B32" s="133"/>
-      <c r="C32" s="131"/>
-      <c r="D32" s="131"/>
-      <c r="E32" s="131"/>
-      <c r="F32" s="131" t="s">
+      <c r="G32" s="105" t="s">
         <v>463</v>
       </c>
-      <c r="G32" s="131" t="s">
-        <v>464</v>
-      </c>
-      <c r="H32" s="131"/>
-      <c r="I32" s="131"/>
-      <c r="J32" s="131"/>
-      <c r="K32" s="131"/>
-      <c r="L32" s="131"/>
-      <c r="M32" s="131"/>
-      <c r="N32" s="131"/>
-      <c r="O32" s="131"/>
-      <c r="P32" s="131"/>
-      <c r="Q32" s="131"/>
-      <c r="R32" s="131"/>
-      <c r="S32" s="131"/>
-      <c r="T32" s="131"/>
-      <c r="U32" s="131"/>
-      <c r="V32" s="131"/>
-      <c r="W32" s="131"/>
-      <c r="X32" s="131"/>
-      <c r="Y32" s="131"/>
-      <c r="Z32" s="131"/>
-      <c r="AA32" s="131"/>
-      <c r="AB32" s="131"/>
-      <c r="AC32" s="131"/>
-      <c r="AD32" s="131"/>
-      <c r="AE32" s="131"/>
-      <c r="AF32" s="131"/>
-      <c r="AG32" s="131"/>
-      <c r="AH32" s="131"/>
-      <c r="AI32" s="131"/>
-      <c r="AJ32" s="131"/>
-      <c r="AK32" s="131"/>
-      <c r="AL32" s="131"/>
-      <c r="AM32" s="131"/>
+      <c r="H32" s="105"/>
+      <c r="I32" s="105"/>
+      <c r="J32" s="105"/>
+      <c r="K32" s="105"/>
+      <c r="L32" s="105"/>
+      <c r="M32" s="105"/>
+      <c r="N32" s="105"/>
+      <c r="O32" s="105"/>
+      <c r="P32" s="105"/>
+      <c r="Q32" s="105"/>
+      <c r="R32" s="105"/>
+      <c r="S32" s="105"/>
+      <c r="T32" s="105"/>
+      <c r="U32" s="105"/>
+      <c r="V32" s="105"/>
+      <c r="W32" s="105"/>
+      <c r="X32" s="105"/>
+      <c r="Y32" s="105"/>
+      <c r="Z32" s="105"/>
+      <c r="AA32" s="105"/>
+      <c r="AB32" s="105"/>
+      <c r="AC32" s="105"/>
+      <c r="AD32" s="105"/>
+      <c r="AE32" s="105"/>
+      <c r="AF32" s="105"/>
+      <c r="AG32" s="105"/>
+      <c r="AH32" s="105"/>
+      <c r="AI32" s="105"/>
+      <c r="AJ32" s="105"/>
+      <c r="AK32" s="105"/>
+      <c r="AL32" s="105"/>
+      <c r="AM32" s="105"/>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A33" s="150" t="s">
+      <c r="A33" s="112" t="s">
         <v>357</v>
       </c>
-      <c r="B33" s="151"/>
-      <c r="C33" s="150"/>
-      <c r="D33" s="150"/>
-      <c r="E33" s="150"/>
-      <c r="F33" s="150"/>
-      <c r="G33" s="150"/>
-      <c r="H33" s="150"/>
-      <c r="I33" s="150"/>
-      <c r="J33" s="150"/>
-      <c r="K33" s="150"/>
-      <c r="L33" s="150"/>
-      <c r="M33" s="150"/>
-      <c r="N33" s="150"/>
-      <c r="O33" s="150"/>
-      <c r="P33" s="150"/>
-      <c r="Q33" s="150"/>
-      <c r="R33" s="150"/>
-      <c r="S33" s="150"/>
-      <c r="T33" s="150"/>
-      <c r="U33" s="150"/>
-      <c r="V33" s="150"/>
-      <c r="W33" s="150"/>
-      <c r="X33" s="150"/>
-      <c r="Y33" s="150"/>
-      <c r="Z33" s="150"/>
-      <c r="AA33" s="150"/>
-      <c r="AB33" s="150"/>
-      <c r="AC33" s="150"/>
-      <c r="AD33" s="150"/>
-      <c r="AE33" s="150"/>
-      <c r="AF33" s="150"/>
-      <c r="AG33" s="150"/>
-      <c r="AH33" s="150"/>
-      <c r="AI33" s="150"/>
-      <c r="AJ33" s="150"/>
-      <c r="AK33" s="150"/>
-      <c r="AL33" s="150"/>
-      <c r="AM33" s="150"/>
+      <c r="B33" s="113"/>
+      <c r="C33" s="112"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="112"/>
+      <c r="G33" s="112"/>
+      <c r="H33" s="112"/>
+      <c r="I33" s="112"/>
+      <c r="J33" s="112"/>
+      <c r="K33" s="112"/>
+      <c r="L33" s="112"/>
+      <c r="M33" s="112"/>
+      <c r="N33" s="112"/>
+      <c r="O33" s="112"/>
+      <c r="P33" s="112"/>
+      <c r="Q33" s="112"/>
+      <c r="R33" s="112"/>
+      <c r="S33" s="112"/>
+      <c r="T33" s="112"/>
+      <c r="U33" s="112"/>
+      <c r="V33" s="112"/>
+      <c r="W33" s="112"/>
+      <c r="X33" s="112"/>
+      <c r="Y33" s="112"/>
+      <c r="Z33" s="112"/>
+      <c r="AA33" s="112"/>
+      <c r="AB33" s="112"/>
+      <c r="AC33" s="112"/>
+      <c r="AD33" s="112"/>
+      <c r="AE33" s="112"/>
+      <c r="AF33" s="112"/>
+      <c r="AG33" s="112"/>
+      <c r="AH33" s="112"/>
+      <c r="AI33" s="112"/>
+      <c r="AJ33" s="112"/>
+      <c r="AK33" s="112"/>
+      <c r="AL33" s="112"/>
+      <c r="AM33" s="112"/>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A34" s="153"/>
-      <c r="B34" s="153"/>
-      <c r="C34" s="153"/>
-      <c r="D34" s="153"/>
-      <c r="E34" s="153"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="153"/>
-      <c r="H34" s="153"/>
-      <c r="I34" s="153"/>
-      <c r="J34" s="153"/>
-      <c r="K34" s="153"/>
-      <c r="L34" s="153"/>
-      <c r="M34" s="153"/>
-      <c r="N34" s="153"/>
-      <c r="O34" s="153"/>
-      <c r="P34" s="153"/>
-      <c r="Q34" s="153"/>
-      <c r="R34" s="153"/>
-      <c r="S34" s="153"/>
-      <c r="T34" s="153"/>
-      <c r="U34" s="153"/>
-      <c r="V34" s="153"/>
-      <c r="W34" s="153"/>
-      <c r="X34" s="153"/>
-      <c r="Y34" s="153"/>
-      <c r="Z34" s="153"/>
-      <c r="AA34" s="153"/>
-      <c r="AB34" s="153"/>
-      <c r="AC34" s="153"/>
-      <c r="AD34" s="153"/>
-      <c r="AE34" s="153"/>
-      <c r="AF34" s="153"/>
-      <c r="AG34" s="153"/>
-      <c r="AH34" s="153"/>
-      <c r="AI34" s="153"/>
-      <c r="AJ34" s="153"/>
-      <c r="AK34" s="153"/>
-      <c r="AL34" s="153"/>
-      <c r="AM34" s="153"/>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A35" s="152"/>
-      <c r="B35" s="152"/>
-      <c r="C35" s="152"/>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="152"/>
-      <c r="H35" s="152"/>
-      <c r="I35" s="152"/>
-      <c r="J35" s="152"/>
-      <c r="K35" s="152"/>
-      <c r="L35" s="152"/>
-      <c r="M35" s="152"/>
-      <c r="N35" s="152"/>
-      <c r="O35" s="152"/>
-      <c r="P35" s="152"/>
-      <c r="Q35" s="152"/>
-      <c r="R35" s="152"/>
-      <c r="S35" s="152"/>
-      <c r="T35" s="152"/>
-      <c r="U35" s="152"/>
-      <c r="V35" s="152"/>
-      <c r="W35" s="152"/>
-      <c r="X35" s="152"/>
-      <c r="Y35" s="152"/>
-      <c r="Z35" s="152"/>
-      <c r="AA35" s="152"/>
-      <c r="AB35" s="152"/>
-      <c r="AC35" s="152"/>
-      <c r="AD35" s="152"/>
-      <c r="AE35" s="152"/>
-      <c r="AF35" s="152"/>
-      <c r="AG35" s="152"/>
-      <c r="AH35" s="152"/>
-      <c r="AI35" s="152"/>
-      <c r="AJ35" s="152"/>
-      <c r="AK35" s="152"/>
-      <c r="AL35" s="152"/>
-      <c r="AM35" s="152"/>
+      <c r="A34" s="114"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="114"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="114"/>
+      <c r="G34" s="114"/>
+      <c r="H34" s="114"/>
+      <c r="I34" s="114"/>
+      <c r="J34" s="114"/>
+      <c r="K34" s="114"/>
+      <c r="L34" s="114"/>
+      <c r="M34" s="114"/>
+      <c r="N34" s="114"/>
+      <c r="O34" s="114"/>
+      <c r="P34" s="114"/>
+      <c r="Q34" s="114"/>
+      <c r="R34" s="114"/>
+      <c r="S34" s="114"/>
+      <c r="T34" s="114"/>
+      <c r="U34" s="114"/>
+      <c r="V34" s="114"/>
+      <c r="W34" s="114"/>
+      <c r="X34" s="114"/>
+      <c r="Y34" s="114"/>
+      <c r="Z34" s="114"/>
+      <c r="AA34" s="114"/>
+      <c r="AB34" s="114"/>
+      <c r="AC34" s="114"/>
+      <c r="AD34" s="114"/>
+      <c r="AE34" s="114"/>
+      <c r="AF34" s="114"/>
+      <c r="AG34" s="114"/>
+      <c r="AH34" s="114"/>
+      <c r="AI34" s="114"/>
+      <c r="AJ34" s="114"/>
+      <c r="AK34" s="114"/>
+      <c r="AL34" s="114"/>
+      <c r="AM34" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C25:C30"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D30"/>
     <mergeCell ref="AF2:AI2"/>
     <mergeCell ref="AJ2:AM2"/>
     <mergeCell ref="A8:A31"/>
@@ -9028,15 +8974,6 @@
     <mergeCell ref="C2:E3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B9:B30"/>
-    <mergeCell ref="C25:C30"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>